<commit_message>
added provider and community listboxes
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCD2CB5-9D6E-4164-80EB-DDBFFF0AC6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855931E0-A27F-47B1-AB69-0AA868692722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="445">
   <si>
     <t>category</t>
   </si>
@@ -2122,15 +2122,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
   <dimension ref="A1:E281"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="C287" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.25" customWidth="1"/>
-    <col min="2" max="2" width="41.75" customWidth="1"/>
-    <col min="3" max="3" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="67.625" customWidth="1"/>
+    <col min="3" max="3" width="64.875" customWidth="1"/>
     <col min="4" max="4" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6561,6 +6561,9 @@
       <c r="B261" t="s">
         <v>426</v>
       </c>
+      <c r="C261" t="s">
+        <v>426</v>
+      </c>
       <c r="D261" t="s">
         <v>8</v>
       </c>
@@ -6575,6 +6578,9 @@
       <c r="B262" t="s">
         <v>427</v>
       </c>
+      <c r="C262" t="s">
+        <v>427</v>
+      </c>
       <c r="D262" t="s">
         <v>8</v>
       </c>
@@ -6589,6 +6595,9 @@
       <c r="B263" t="s">
         <v>428</v>
       </c>
+      <c r="C263" t="s">
+        <v>428</v>
+      </c>
       <c r="D263" t="s">
         <v>8</v>
       </c>
@@ -6603,6 +6612,9 @@
       <c r="B264" t="s">
         <v>429</v>
       </c>
+      <c r="C264" t="s">
+        <v>429</v>
+      </c>
       <c r="D264" t="s">
         <v>8</v>
       </c>
@@ -6617,6 +6629,9 @@
       <c r="B265" t="s">
         <v>431</v>
       </c>
+      <c r="C265" t="s">
+        <v>431</v>
+      </c>
       <c r="D265" t="s">
         <v>8</v>
       </c>
@@ -6631,7 +6646,9 @@
       <c r="B266" t="s">
         <v>432</v>
       </c>
-      <c r="C266" s="1"/>
+      <c r="C266" t="s">
+        <v>432</v>
+      </c>
       <c r="D266" t="s">
         <v>8</v>
       </c>
@@ -6646,6 +6663,9 @@
       <c r="B267" t="s">
         <v>433</v>
       </c>
+      <c r="C267" t="s">
+        <v>433</v>
+      </c>
       <c r="D267" t="s">
         <v>8</v>
       </c>
@@ -6660,6 +6680,9 @@
       <c r="B268" t="s">
         <v>434</v>
       </c>
+      <c r="C268" t="s">
+        <v>434</v>
+      </c>
       <c r="D268" t="s">
         <v>8</v>
       </c>
@@ -6674,6 +6697,9 @@
       <c r="B269" t="s">
         <v>435</v>
       </c>
+      <c r="C269" t="s">
+        <v>435</v>
+      </c>
       <c r="D269" t="s">
         <v>8</v>
       </c>
@@ -6688,6 +6714,9 @@
       <c r="B270" t="s">
         <v>436</v>
       </c>
+      <c r="C270" t="s">
+        <v>436</v>
+      </c>
       <c r="D270" t="s">
         <v>8</v>
       </c>
@@ -6702,6 +6731,9 @@
       <c r="B271" t="s">
         <v>437</v>
       </c>
+      <c r="C271" t="s">
+        <v>437</v>
+      </c>
       <c r="D271" t="s">
         <v>8</v>
       </c>
@@ -6716,6 +6748,9 @@
       <c r="B272" t="s">
         <v>438</v>
       </c>
+      <c r="C272" t="s">
+        <v>438</v>
+      </c>
       <c r="D272" t="s">
         <v>8</v>
       </c>
@@ -6730,6 +6765,9 @@
       <c r="B273" t="s">
         <v>439</v>
       </c>
+      <c r="C273" t="s">
+        <v>439</v>
+      </c>
       <c r="D273" t="s">
         <v>8</v>
       </c>
@@ -6744,6 +6782,9 @@
       <c r="B274" s="3" t="s">
         <v>441</v>
       </c>
+      <c r="C274" s="3" t="s">
+        <v>441</v>
+      </c>
       <c r="D274" t="s">
         <v>8</v>
       </c>
@@ -6758,6 +6799,9 @@
       <c r="B275" s="3" t="s">
         <v>442</v>
       </c>
+      <c r="C275" s="3" t="s">
+        <v>442</v>
+      </c>
       <c r="D275" t="s">
         <v>8</v>
       </c>
@@ -6772,6 +6816,9 @@
       <c r="B276" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="C276" s="3" t="s">
+        <v>443</v>
+      </c>
       <c r="D276" t="s">
         <v>8</v>
       </c>
@@ -6786,6 +6833,9 @@
       <c r="B277" s="3" t="s">
         <v>444</v>
       </c>
+      <c r="C277" s="3" t="s">
+        <v>444</v>
+      </c>
       <c r="D277" t="s">
         <v>8</v>
       </c>
@@ -6800,6 +6850,9 @@
       <c r="B278" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="C278" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D278" t="s">
         <v>8</v>
       </c>
@@ -6814,6 +6867,9 @@
       <c r="B279" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="C279" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="D279" t="s">
         <v>8</v>
       </c>
@@ -6828,6 +6884,9 @@
       <c r="B280" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="C280" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D280" t="s">
         <v>8</v>
       </c>
@@ -6842,6 +6901,9 @@
       <c r="B281" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="C281" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="D281" t="s">
         <v>8</v>
       </c>
@@ -6851,5 +6913,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added delete db script
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640E71B-6BCB-486D-B82C-0A7A1350E161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C336D64-9D00-4DA9-B583-C1BE6B5689FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
+    <workbookView xWindow="810" yWindow="16080" windowWidth="28110" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="469">
   <si>
     <t>category</t>
   </si>
@@ -794,9 +794,6 @@
     <t>My family has enough income to purchase basic clothing.</t>
   </si>
   <si>
-    <t>New skills</t>
-  </si>
-  <si>
     <t>In what sense do you think you learned new skills in the past 6 months?</t>
   </si>
   <si>
@@ -1809,6 +1806,15 @@
   </si>
   <si>
     <t>E-mail; News/entertainment; Business transactions/banking; General search for information; Academic (learning, teaching, research)</t>
+  </si>
+  <si>
+    <t>Repeater ratio</t>
+  </si>
+  <si>
+    <t>New skills 1</t>
+  </si>
+  <si>
+    <t>New skills 2</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,13 +2225,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -2236,13 +2242,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H2" t="s">
         <v>80</v>
@@ -2253,13 +2259,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H3" t="s">
         <v>80</v>
@@ -2270,13 +2276,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H4" t="s">
         <v>80</v>
@@ -2287,13 +2293,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H5" t="s">
         <v>80</v>
@@ -2304,13 +2310,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H6" t="s">
         <v>80</v>
@@ -2327,7 +2333,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H7" t="s">
         <v>80</v>
@@ -2344,7 +2350,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H8" t="s">
         <v>80</v>
@@ -2361,7 +2367,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H9" t="s">
         <v>80</v>
@@ -2378,7 +2384,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H10" t="s">
         <v>80</v>
@@ -2395,7 +2401,7 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H11" t="s">
         <v>80</v>
@@ -2412,7 +2418,7 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H12" t="s">
         <v>80</v>
@@ -2429,7 +2435,7 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H13" t="s">
         <v>80</v>
@@ -2446,7 +2452,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H14" t="s">
         <v>80</v>
@@ -2463,7 +2469,7 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H15" t="s">
         <v>80</v>
@@ -2480,7 +2486,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H16" t="s">
         <v>80</v>
@@ -2497,7 +2503,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H17" t="s">
         <v>80</v>
@@ -2508,13 +2514,13 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H18" t="s">
         <v>80</v>
@@ -2525,13 +2531,13 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C19" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
@@ -2542,13 +2548,13 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H20" t="s">
         <v>80</v>
@@ -2559,13 +2565,13 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C21" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H21" t="s">
         <v>80</v>
@@ -2576,13 +2582,13 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H22" t="s">
         <v>80</v>
@@ -2593,13 +2599,13 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H23" t="s">
         <v>80</v>
@@ -2610,13 +2616,13 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C24" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H24" t="s">
         <v>80</v>
@@ -2627,13 +2633,13 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H25" t="s">
         <v>80</v>
@@ -2644,13 +2650,13 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C26" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H26" t="s">
         <v>80</v>
@@ -2667,7 +2673,7 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H27" t="s">
         <v>80</v>
@@ -2684,7 +2690,7 @@
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H28" t="s">
         <v>80</v>
@@ -2695,13 +2701,13 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>466</v>
       </c>
       <c r="C29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H29" t="s">
         <v>80</v>
@@ -2712,13 +2718,13 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H30" t="s">
         <v>80</v>
@@ -2729,13 +2735,13 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H31" t="s">
         <v>80</v>
@@ -2746,13 +2752,13 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H32" t="s">
         <v>80</v>
@@ -2763,13 +2769,13 @@
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C33" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H33" t="s">
         <v>80</v>
@@ -2786,7 +2792,7 @@
         <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H34" t="s">
         <v>80</v>
@@ -2803,7 +2809,7 @@
         <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H35" t="s">
         <v>80</v>
@@ -2820,7 +2826,7 @@
         <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H36" t="s">
         <v>80</v>
@@ -2837,7 +2843,7 @@
         <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H37" t="s">
         <v>80</v>
@@ -2854,7 +2860,7 @@
         <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H38" t="s">
         <v>80</v>
@@ -2865,13 +2871,13 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D39" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H39" t="s">
         <v>80</v>
@@ -2888,7 +2894,7 @@
         <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H40" t="s">
         <v>80</v>
@@ -2905,7 +2911,7 @@
         <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H41" t="s">
         <v>80</v>
@@ -2919,16 +2925,16 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D42" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E42" s="5">
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H42" t="s">
         <v>80</v>
@@ -2942,16 +2948,16 @@
         <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D43" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E43" s="5">
         <v>4</v>
       </c>
       <c r="G43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H43" t="s">
         <v>80</v>
@@ -2962,13 +2968,13 @@
         <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H44" t="s">
         <v>80</v>
@@ -2985,7 +2991,7 @@
         <v>64</v>
       </c>
       <c r="D45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H45" t="s">
         <v>80</v>
@@ -3002,7 +3008,7 @@
         <v>66</v>
       </c>
       <c r="D46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H46" t="s">
         <v>80</v>
@@ -3019,7 +3025,7 @@
         <v>68</v>
       </c>
       <c r="D47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H47" t="s">
         <v>80</v>
@@ -3036,7 +3042,7 @@
         <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H48" t="s">
         <v>80</v>
@@ -3053,7 +3059,7 @@
         <v>72</v>
       </c>
       <c r="D49" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H49" t="s">
         <v>80</v>
@@ -3070,7 +3076,7 @@
         <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H50" t="s">
         <v>80</v>
@@ -3087,7 +3093,7 @@
         <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H51" t="s">
         <v>80</v>
@@ -3098,13 +3104,13 @@
         <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C52" t="s">
         <v>78</v>
       </c>
       <c r="D52" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H52" t="s">
         <v>80</v>
@@ -3115,13 +3121,13 @@
         <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C53" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D53" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H53" t="s">
         <v>80</v>
@@ -3138,10 +3144,10 @@
         <v>84</v>
       </c>
       <c r="D54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3155,16 +3161,16 @@
         <v>86</v>
       </c>
       <c r="D55" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E55" s="5">
         <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3181,7 +3187,7 @@
         <v>89</v>
       </c>
       <c r="H56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3198,7 +3204,7 @@
         <v>89</v>
       </c>
       <c r="H57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3215,7 +3221,7 @@
         <v>89</v>
       </c>
       <c r="H58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3232,7 +3238,7 @@
         <v>89</v>
       </c>
       <c r="H59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3246,16 +3252,16 @@
         <v>97</v>
       </c>
       <c r="D60" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E60" s="5">
         <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3263,16 +3269,16 @@
         <v>82</v>
       </c>
       <c r="B61" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C61" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D61" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3280,16 +3286,16 @@
         <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C62" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D62" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3300,7 +3306,7 @@
         <v>99</v>
       </c>
       <c r="C63" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D63" t="s">
         <v>60</v>
@@ -3309,10 +3315,10 @@
         <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3323,7 +3329,7 @@
         <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D64" t="s">
         <v>60</v>
@@ -3332,10 +3338,10 @@
         <v>6</v>
       </c>
       <c r="G64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3349,10 +3355,10 @@
         <v>103</v>
       </c>
       <c r="D65" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H65" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3363,19 +3369,19 @@
         <v>104</v>
       </c>
       <c r="C66" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D66" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E66" s="5">
         <v>5</v>
       </c>
       <c r="G66" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H66" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3383,16 +3389,16 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
       </c>
       <c r="D67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H67" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3406,10 +3412,10 @@
         <v>107</v>
       </c>
       <c r="D68" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H68" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3423,10 +3429,10 @@
         <v>109</v>
       </c>
       <c r="D69" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H69" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3437,19 +3443,19 @@
         <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D70" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E70" s="5">
         <v>4</v>
       </c>
       <c r="G70" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3460,22 +3466,22 @@
         <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D71" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E71" s="5">
         <v>5</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G71" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,19 +3492,19 @@
         <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D72" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E72" s="5">
         <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H72" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3509,19 +3515,19 @@
         <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D73" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E73" s="5">
         <v>4</v>
       </c>
       <c r="G73" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3532,19 +3538,19 @@
         <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D74" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E74" s="5">
         <v>4</v>
       </c>
       <c r="G74" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3555,19 +3561,19 @@
         <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D75" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E75" s="5">
         <v>4</v>
       </c>
       <c r="G75" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,10 +3587,10 @@
         <v>118</v>
       </c>
       <c r="D76" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3598,10 +3604,10 @@
         <v>120</v>
       </c>
       <c r="D77" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H77" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3612,22 +3618,22 @@
         <v>121</v>
       </c>
       <c r="C78" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D78" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E78" s="5">
         <v>5</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G78" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3641,10 +3647,10 @@
         <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H79" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3658,10 +3664,10 @@
         <v>126</v>
       </c>
       <c r="D80" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3672,22 +3678,22 @@
         <v>127</v>
       </c>
       <c r="C81" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D81" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E81" s="5">
         <v>5</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G81" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H81" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3701,10 +3707,10 @@
         <v>16</v>
       </c>
       <c r="D82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H82" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3718,10 +3724,10 @@
         <v>18</v>
       </c>
       <c r="D83" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3738,7 +3744,7 @@
         <v>130</v>
       </c>
       <c r="H84" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3755,7 +3761,7 @@
         <v>130</v>
       </c>
       <c r="H85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3772,7 +3778,7 @@
         <v>130</v>
       </c>
       <c r="H86" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3789,7 +3795,7 @@
         <v>130</v>
       </c>
       <c r="H87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3806,7 +3812,7 @@
         <v>130</v>
       </c>
       <c r="H88" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3823,7 +3829,7 @@
         <v>130</v>
       </c>
       <c r="H89" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3840,7 +3846,7 @@
         <v>130</v>
       </c>
       <c r="H90" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3857,7 +3863,7 @@
         <v>130</v>
       </c>
       <c r="H91" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3868,13 +3874,13 @@
         <v>146</v>
       </c>
       <c r="C92" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D92" t="s">
         <v>130</v>
       </c>
       <c r="H92" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3891,7 +3897,7 @@
         <v>130</v>
       </c>
       <c r="H93" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3908,7 +3914,7 @@
         <v>130</v>
       </c>
       <c r="H94" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3925,7 +3931,7 @@
         <v>130</v>
       </c>
       <c r="H95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3942,7 +3948,7 @@
         <v>130</v>
       </c>
       <c r="H96" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3959,7 +3965,7 @@
         <v>130</v>
       </c>
       <c r="H97" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3976,7 +3982,7 @@
         <v>130</v>
       </c>
       <c r="H98" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3987,13 +3993,13 @@
         <v>159</v>
       </c>
       <c r="C99" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D99" t="s">
         <v>130</v>
       </c>
       <c r="H99" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4010,7 +4016,7 @@
         <v>130</v>
       </c>
       <c r="H100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4027,7 +4033,7 @@
         <v>130</v>
       </c>
       <c r="H101" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4044,7 +4050,7 @@
         <v>130</v>
       </c>
       <c r="H102" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4061,7 +4067,7 @@
         <v>130</v>
       </c>
       <c r="H103" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4078,7 +4084,7 @@
         <v>130</v>
       </c>
       <c r="H104" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4095,7 +4101,7 @@
         <v>130</v>
       </c>
       <c r="H105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4112,7 +4118,7 @@
         <v>130</v>
       </c>
       <c r="H106" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4129,7 +4135,7 @@
         <v>130</v>
       </c>
       <c r="H107" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4146,7 +4152,7 @@
         <v>130</v>
       </c>
       <c r="H108" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4163,7 +4169,7 @@
         <v>130</v>
       </c>
       <c r="H109" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4180,7 +4186,7 @@
         <v>130</v>
       </c>
       <c r="H110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4197,7 +4203,7 @@
         <v>130</v>
       </c>
       <c r="H111" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4214,7 +4220,7 @@
         <v>130</v>
       </c>
       <c r="H112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4231,7 +4237,7 @@
         <v>130</v>
       </c>
       <c r="H113" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4248,7 +4254,7 @@
         <v>130</v>
       </c>
       <c r="H114" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4265,7 +4271,7 @@
         <v>130</v>
       </c>
       <c r="H115" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4282,7 +4288,7 @@
         <v>130</v>
       </c>
       <c r="H116" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4299,7 +4305,7 @@
         <v>130</v>
       </c>
       <c r="H117" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4316,7 +4322,7 @@
         <v>130</v>
       </c>
       <c r="H118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4333,7 +4339,7 @@
         <v>130</v>
       </c>
       <c r="H119" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4350,7 +4356,7 @@
         <v>130</v>
       </c>
       <c r="H120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4367,7 +4373,7 @@
         <v>130</v>
       </c>
       <c r="H121" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4384,7 +4390,7 @@
         <v>130</v>
       </c>
       <c r="H122" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4401,7 +4407,7 @@
         <v>130</v>
       </c>
       <c r="H123" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4418,7 +4424,7 @@
         <v>130</v>
       </c>
       <c r="H124" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4435,7 +4441,7 @@
         <v>130</v>
       </c>
       <c r="H125" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4452,7 +4458,7 @@
         <v>130</v>
       </c>
       <c r="H126" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4469,7 +4475,7 @@
         <v>130</v>
       </c>
       <c r="H127" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4486,7 +4492,7 @@
         <v>130</v>
       </c>
       <c r="H128" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4503,7 +4509,7 @@
         <v>130</v>
       </c>
       <c r="H129" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4520,7 +4526,7 @@
         <v>130</v>
       </c>
       <c r="H130" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4537,7 +4543,7 @@
         <v>130</v>
       </c>
       <c r="H131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4554,7 +4560,7 @@
         <v>130</v>
       </c>
       <c r="H132" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4568,10 +4574,10 @@
         <v>220</v>
       </c>
       <c r="D133" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H133" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4585,10 +4591,10 @@
         <v>222</v>
       </c>
       <c r="D134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H134" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4605,7 +4611,7 @@
         <v>130</v>
       </c>
       <c r="H135" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4622,7 +4628,7 @@
         <v>130</v>
       </c>
       <c r="H136" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4639,7 +4645,7 @@
         <v>130</v>
       </c>
       <c r="H137" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4656,7 +4662,7 @@
         <v>130</v>
       </c>
       <c r="H138" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4673,7 +4679,7 @@
         <v>130</v>
       </c>
       <c r="H139" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4690,7 +4696,7 @@
         <v>130</v>
       </c>
       <c r="H140" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4707,7 +4713,7 @@
         <v>130</v>
       </c>
       <c r="H141" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -4715,16 +4721,16 @@
         <v>229</v>
       </c>
       <c r="B142" t="s">
+        <v>467</v>
+      </c>
+      <c r="C142" t="s">
         <v>238</v>
       </c>
-      <c r="C142" t="s">
-        <v>239</v>
-      </c>
       <c r="D142" t="s">
         <v>130</v>
       </c>
       <c r="H142" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -4732,22 +4738,22 @@
         <v>229</v>
       </c>
       <c r="B143" t="s">
-        <v>238</v>
+        <v>468</v>
       </c>
       <c r="C143" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D143" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E143" s="5">
         <v>3</v>
       </c>
       <c r="G143" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H143" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -4755,16 +4761,16 @@
         <v>229</v>
       </c>
       <c r="B144" t="s">
+        <v>239</v>
+      </c>
+      <c r="C144" t="s">
         <v>240</v>
       </c>
-      <c r="C144" t="s">
-        <v>241</v>
-      </c>
       <c r="D144" t="s">
         <v>130</v>
       </c>
       <c r="H144" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -4772,16 +4778,16 @@
         <v>229</v>
       </c>
       <c r="B145" t="s">
+        <v>241</v>
+      </c>
+      <c r="C145" t="s">
         <v>242</v>
       </c>
-      <c r="C145" t="s">
-        <v>243</v>
-      </c>
       <c r="D145" t="s">
         <v>130</v>
       </c>
       <c r="H145" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -4789,16 +4795,16 @@
         <v>229</v>
       </c>
       <c r="B146" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146" t="s">
         <v>244</v>
       </c>
-      <c r="C146" t="s">
-        <v>245</v>
-      </c>
       <c r="D146" t="s">
         <v>130</v>
       </c>
       <c r="H146" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -4812,10 +4818,10 @@
         <v>84</v>
       </c>
       <c r="D147" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H147" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -4829,16 +4835,16 @@
         <v>86</v>
       </c>
       <c r="D148" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E148" s="5">
         <v>2</v>
       </c>
       <c r="G148" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H148" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -4855,7 +4861,7 @@
         <v>89</v>
       </c>
       <c r="H149" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -4872,7 +4878,7 @@
         <v>89</v>
       </c>
       <c r="H150" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -4883,13 +4889,13 @@
         <v>92</v>
       </c>
       <c r="C151" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D151" t="s">
         <v>89</v>
       </c>
       <c r="H151" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -4906,7 +4912,7 @@
         <v>89</v>
       </c>
       <c r="H152" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -4923,7 +4929,7 @@
         <v>60</v>
       </c>
       <c r="H153" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -4931,16 +4937,16 @@
         <v>82</v>
       </c>
       <c r="B154" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C154" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D154" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H154" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -4948,16 +4954,16 @@
         <v>82</v>
       </c>
       <c r="B155" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C155" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D155" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H155" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -4968,7 +4974,7 @@
         <v>99</v>
       </c>
       <c r="C156" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D156" t="s">
         <v>60</v>
@@ -4977,10 +4983,10 @@
         <v>7</v>
       </c>
       <c r="G156" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H156" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -4988,10 +4994,10 @@
         <v>98</v>
       </c>
       <c r="B157" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C157" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D157" t="s">
         <v>60</v>
@@ -5000,10 +5006,10 @@
         <v>6</v>
       </c>
       <c r="G157" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H157" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5017,10 +5023,10 @@
         <v>103</v>
       </c>
       <c r="D158" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H158" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5031,19 +5037,19 @@
         <v>104</v>
       </c>
       <c r="C159" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D159" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E159" s="5">
         <v>5</v>
       </c>
       <c r="G159" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H159" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5051,16 +5057,16 @@
         <v>58</v>
       </c>
       <c r="B160" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C160" t="s">
         <v>105</v>
       </c>
       <c r="D160" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H160" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5071,13 +5077,13 @@
         <v>106</v>
       </c>
       <c r="C161" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D161" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H161" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -5091,10 +5097,10 @@
         <v>109</v>
       </c>
       <c r="D162" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H162" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -5105,19 +5111,19 @@
         <v>110</v>
       </c>
       <c r="C163" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D163" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E163" s="5">
         <v>4</v>
       </c>
       <c r="G163" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H163" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -5128,22 +5134,22 @@
         <v>111</v>
       </c>
       <c r="C164" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D164" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E164" s="5">
         <v>5</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G164" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H164" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -5154,19 +5160,19 @@
         <v>112</v>
       </c>
       <c r="C165" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D165" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E165" s="5">
         <v>5</v>
       </c>
       <c r="G165" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H165" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -5174,22 +5180,22 @@
         <v>79</v>
       </c>
       <c r="B166" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C166" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D166" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E166" s="5">
         <v>4</v>
       </c>
       <c r="G166" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H166" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -5200,19 +5206,19 @@
         <v>114</v>
       </c>
       <c r="C167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D167" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E167" s="5">
         <v>4</v>
       </c>
       <c r="G167" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H167" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -5223,19 +5229,19 @@
         <v>115</v>
       </c>
       <c r="C168" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D168" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E168" s="5">
         <v>4</v>
       </c>
       <c r="G168" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H168" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -5249,10 +5255,10 @@
         <v>118</v>
       </c>
       <c r="D169" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H169" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -5266,10 +5272,10 @@
         <v>120</v>
       </c>
       <c r="D170" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H170" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -5280,22 +5286,22 @@
         <v>121</v>
       </c>
       <c r="C171" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D171" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E171" s="5">
         <v>5</v>
       </c>
       <c r="F171" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G171" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H171" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -5309,10 +5315,10 @@
         <v>124</v>
       </c>
       <c r="D172" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H172" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -5326,10 +5332,10 @@
         <v>126</v>
       </c>
       <c r="D173" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H173" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -5340,22 +5346,22 @@
         <v>127</v>
       </c>
       <c r="C174" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D174" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E174" s="5">
         <v>5</v>
       </c>
       <c r="F174" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G174" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H174" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -5369,10 +5375,10 @@
         <v>16</v>
       </c>
       <c r="D175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H175" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -5386,10 +5392,10 @@
         <v>18</v>
       </c>
       <c r="D176" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H176" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -5397,16 +5403,16 @@
         <v>96</v>
       </c>
       <c r="B177" t="s">
+        <v>249</v>
+      </c>
+      <c r="C177" t="s">
         <v>250</v>
       </c>
-      <c r="C177" t="s">
-        <v>251</v>
-      </c>
       <c r="D177" t="s">
         <v>130</v>
       </c>
       <c r="H177" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -5414,16 +5420,16 @@
         <v>137</v>
       </c>
       <c r="B178" t="s">
+        <v>251</v>
+      </c>
+      <c r="C178" t="s">
         <v>252</v>
       </c>
-      <c r="C178" t="s">
-        <v>253</v>
-      </c>
       <c r="D178" t="s">
         <v>130</v>
       </c>
       <c r="H178" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -5431,16 +5437,16 @@
         <v>137</v>
       </c>
       <c r="B179" t="s">
+        <v>253</v>
+      </c>
+      <c r="C179" t="s">
         <v>254</v>
       </c>
-      <c r="C179" t="s">
-        <v>255</v>
-      </c>
       <c r="D179" t="s">
         <v>130</v>
       </c>
       <c r="H179" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -5448,16 +5454,16 @@
         <v>137</v>
       </c>
       <c r="B180" t="s">
+        <v>255</v>
+      </c>
+      <c r="C180" t="s">
         <v>256</v>
       </c>
-      <c r="C180" t="s">
-        <v>257</v>
-      </c>
       <c r="D180" t="s">
         <v>130</v>
       </c>
       <c r="H180" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -5465,16 +5471,16 @@
         <v>137</v>
       </c>
       <c r="B181" t="s">
+        <v>257</v>
+      </c>
+      <c r="C181" t="s">
         <v>258</v>
       </c>
-      <c r="C181" t="s">
-        <v>259</v>
-      </c>
       <c r="D181" t="s">
         <v>130</v>
       </c>
       <c r="H181" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -5491,7 +5497,7 @@
         <v>130</v>
       </c>
       <c r="H182" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -5502,13 +5508,13 @@
         <v>142</v>
       </c>
       <c r="C183" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D183" t="s">
         <v>130</v>
       </c>
       <c r="H183" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -5519,13 +5525,13 @@
         <v>144</v>
       </c>
       <c r="C184" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D184" t="s">
         <v>130</v>
       </c>
       <c r="H184" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -5536,13 +5542,13 @@
         <v>146</v>
       </c>
       <c r="C185" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D185" t="s">
         <v>130</v>
       </c>
       <c r="H185" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -5559,7 +5565,7 @@
         <v>130</v>
       </c>
       <c r="H186" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -5576,7 +5582,7 @@
         <v>130</v>
       </c>
       <c r="H187" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -5587,13 +5593,13 @@
         <v>151</v>
       </c>
       <c r="C188" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D188" t="s">
         <v>130</v>
       </c>
       <c r="H188" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -5604,13 +5610,13 @@
         <v>153</v>
       </c>
       <c r="C189" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D189" t="s">
         <v>130</v>
       </c>
       <c r="H189" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -5621,13 +5627,13 @@
         <v>155</v>
       </c>
       <c r="C190" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D190" t="s">
         <v>130</v>
       </c>
       <c r="H190" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -5644,7 +5650,7 @@
         <v>130</v>
       </c>
       <c r="H191" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -5655,13 +5661,13 @@
         <v>159</v>
       </c>
       <c r="C192" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D192" t="s">
         <v>130</v>
       </c>
       <c r="H192" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -5669,7 +5675,7 @@
         <v>62</v>
       </c>
       <c r="B193" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C193" t="s">
         <v>161</v>
@@ -5678,7 +5684,7 @@
         <v>130</v>
       </c>
       <c r="H193" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -5686,7 +5692,7 @@
         <v>62</v>
       </c>
       <c r="B194" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C194" t="s">
         <v>163</v>
@@ -5695,7 +5701,7 @@
         <v>130</v>
       </c>
       <c r="H194" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -5703,16 +5709,16 @@
         <v>62</v>
       </c>
       <c r="B195" t="s">
+        <v>266</v>
+      </c>
+      <c r="C195" t="s">
         <v>267</v>
       </c>
-      <c r="C195" t="s">
-        <v>268</v>
-      </c>
       <c r="D195" t="s">
         <v>130</v>
       </c>
       <c r="H195" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -5729,7 +5735,7 @@
         <v>130</v>
       </c>
       <c r="H196" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -5746,7 +5752,7 @@
         <v>130</v>
       </c>
       <c r="H197" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -5754,7 +5760,7 @@
         <v>122</v>
       </c>
       <c r="B198" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C198" t="s">
         <v>184</v>
@@ -5763,7 +5769,7 @@
         <v>130</v>
       </c>
       <c r="H198" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -5780,211 +5786,211 @@
         <v>130</v>
       </c>
       <c r="H199" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B200" t="s">
+        <v>269</v>
+      </c>
+      <c r="C200" t="s">
         <v>270</v>
       </c>
-      <c r="C200" t="s">
-        <v>271</v>
-      </c>
       <c r="D200" t="s">
         <v>130</v>
       </c>
       <c r="H200" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>271</v>
+      </c>
+      <c r="B201" t="s">
         <v>272</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>273</v>
       </c>
-      <c r="C201" t="s">
-        <v>274</v>
-      </c>
       <c r="D201" t="s">
         <v>130</v>
       </c>
       <c r="H201" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B202" t="s">
+        <v>274</v>
+      </c>
+      <c r="C202" t="s">
         <v>275</v>
       </c>
-      <c r="C202" t="s">
-        <v>276</v>
-      </c>
       <c r="D202" t="s">
         <v>130</v>
       </c>
       <c r="H202" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B203" t="s">
+        <v>276</v>
+      </c>
+      <c r="C203" t="s">
         <v>277</v>
       </c>
-      <c r="C203" t="s">
-        <v>278</v>
-      </c>
       <c r="D203" t="s">
         <v>130</v>
       </c>
       <c r="H203" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B204" t="s">
+        <v>278</v>
+      </c>
+      <c r="C204" t="s">
         <v>279</v>
       </c>
-      <c r="C204" t="s">
-        <v>280</v>
-      </c>
       <c r="D204" t="s">
         <v>130</v>
       </c>
       <c r="H204" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B205" t="s">
+        <v>280</v>
+      </c>
+      <c r="C205" t="s">
         <v>281</v>
       </c>
-      <c r="C205" t="s">
-        <v>282</v>
-      </c>
       <c r="D205" t="s">
         <v>130</v>
       </c>
       <c r="H205" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B206" t="s">
+        <v>282</v>
+      </c>
+      <c r="C206" t="s">
         <v>283</v>
       </c>
-      <c r="C206" t="s">
-        <v>284</v>
-      </c>
       <c r="D206" t="s">
         <v>130</v>
       </c>
       <c r="H206" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B207" t="s">
+        <v>284</v>
+      </c>
+      <c r="C207" t="s">
         <v>285</v>
       </c>
-      <c r="C207" t="s">
-        <v>286</v>
-      </c>
       <c r="D207" t="s">
         <v>130</v>
       </c>
       <c r="H207" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B208" t="s">
+        <v>286</v>
+      </c>
+      <c r="C208" t="s">
         <v>287</v>
       </c>
-      <c r="C208" t="s">
-        <v>288</v>
-      </c>
       <c r="D208" t="s">
         <v>130</v>
       </c>
       <c r="H208" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B209" t="s">
+        <v>288</v>
+      </c>
+      <c r="C209" t="s">
         <v>289</v>
       </c>
-      <c r="C209" t="s">
-        <v>290</v>
-      </c>
       <c r="D209" t="s">
         <v>130</v>
       </c>
       <c r="H209" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B210" t="s">
+        <v>290</v>
+      </c>
+      <c r="C210" t="s">
         <v>291</v>
       </c>
-      <c r="C210" t="s">
-        <v>292</v>
-      </c>
       <c r="D210" t="s">
         <v>130</v>
       </c>
       <c r="H210" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B211" t="s">
+        <v>292</v>
+      </c>
+      <c r="C211" t="s">
         <v>293</v>
       </c>
-      <c r="C211" t="s">
-        <v>294</v>
-      </c>
       <c r="D211" t="s">
         <v>130</v>
       </c>
       <c r="H211" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -6001,7 +6007,7 @@
         <v>130</v>
       </c>
       <c r="H212" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -6018,7 +6024,7 @@
         <v>130</v>
       </c>
       <c r="H213" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -6035,7 +6041,7 @@
         <v>130</v>
       </c>
       <c r="H214" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -6052,7 +6058,7 @@
         <v>130</v>
       </c>
       <c r="H215" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -6069,7 +6075,7 @@
         <v>130</v>
       </c>
       <c r="H216" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -6086,7 +6092,7 @@
         <v>130</v>
       </c>
       <c r="H217" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -6103,7 +6109,7 @@
         <v>130</v>
       </c>
       <c r="H218" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -6120,7 +6126,7 @@
         <v>130</v>
       </c>
       <c r="H219" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -6137,7 +6143,7 @@
         <v>130</v>
       </c>
       <c r="H220" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -6154,7 +6160,7 @@
         <v>130</v>
       </c>
       <c r="H221" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -6171,7 +6177,7 @@
         <v>130</v>
       </c>
       <c r="H222" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -6188,7 +6194,7 @@
         <v>130</v>
       </c>
       <c r="H223" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -6205,7 +6211,7 @@
         <v>130</v>
       </c>
       <c r="H224" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -6222,7 +6228,7 @@
         <v>130</v>
       </c>
       <c r="H225" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -6239,7 +6245,7 @@
         <v>130</v>
       </c>
       <c r="H226" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -6256,7 +6262,7 @@
         <v>130</v>
       </c>
       <c r="H227" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -6273,7 +6279,7 @@
         <v>130</v>
       </c>
       <c r="H228" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -6290,548 +6296,548 @@
         <v>130</v>
       </c>
       <c r="H229" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>294</v>
+      </c>
+      <c r="B230" t="s">
         <v>295</v>
       </c>
-      <c r="B230" t="s">
+      <c r="C230" t="s">
         <v>296</v>
       </c>
-      <c r="C230" t="s">
-        <v>297</v>
-      </c>
       <c r="D230" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H230" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B231" t="s">
+        <v>297</v>
+      </c>
+      <c r="C231" t="s">
         <v>298</v>
       </c>
-      <c r="C231" t="s">
-        <v>299</v>
-      </c>
       <c r="D231" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H231" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B232" t="s">
+        <v>299</v>
+      </c>
+      <c r="C232" t="s">
         <v>300</v>
       </c>
-      <c r="C232" t="s">
-        <v>301</v>
-      </c>
       <c r="D232" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H232" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B233" t="s">
+        <v>301</v>
+      </c>
+      <c r="C233" t="s">
         <v>302</v>
       </c>
-      <c r="C233" t="s">
-        <v>303</v>
-      </c>
       <c r="D233" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H233" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B234" t="s">
+        <v>303</v>
+      </c>
+      <c r="C234" t="s">
         <v>304</v>
       </c>
-      <c r="C234" t="s">
-        <v>305</v>
-      </c>
       <c r="D234" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H234" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B235" t="s">
+        <v>305</v>
+      </c>
+      <c r="C235" t="s">
         <v>306</v>
       </c>
-      <c r="C235" t="s">
-        <v>307</v>
-      </c>
       <c r="D235" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H235" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B236" t="s">
+        <v>307</v>
+      </c>
+      <c r="C236" t="s">
         <v>308</v>
       </c>
-      <c r="C236" t="s">
-        <v>309</v>
-      </c>
       <c r="D236" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H236" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B237" t="s">
+        <v>309</v>
+      </c>
+      <c r="C237" t="s">
         <v>310</v>
       </c>
-      <c r="C237" t="s">
-        <v>311</v>
-      </c>
       <c r="D237" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H237" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B238" t="s">
+        <v>311</v>
+      </c>
+      <c r="C238" t="s">
         <v>312</v>
       </c>
-      <c r="C238" t="s">
-        <v>313</v>
-      </c>
       <c r="D238" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H238" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B239" t="s">
+        <v>313</v>
+      </c>
+      <c r="C239" t="s">
         <v>314</v>
       </c>
-      <c r="C239" t="s">
-        <v>315</v>
-      </c>
       <c r="D239" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H239" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B240" t="s">
+        <v>315</v>
+      </c>
+      <c r="C240" t="s">
         <v>316</v>
       </c>
-      <c r="C240" t="s">
-        <v>317</v>
-      </c>
       <c r="D240" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H240" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B241" t="s">
+        <v>317</v>
+      </c>
+      <c r="C241" t="s">
         <v>318</v>
       </c>
-      <c r="C241" t="s">
-        <v>319</v>
-      </c>
       <c r="D241" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H241" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B242" t="s">
+        <v>319</v>
+      </c>
+      <c r="C242" t="s">
         <v>320</v>
       </c>
-      <c r="C242" t="s">
-        <v>321</v>
-      </c>
       <c r="D242" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H242" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B243" t="s">
+        <v>321</v>
+      </c>
+      <c r="C243" t="s">
         <v>322</v>
       </c>
-      <c r="C243" t="s">
-        <v>323</v>
-      </c>
       <c r="D243" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H243" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B244" t="s">
+        <v>323</v>
+      </c>
+      <c r="C244" t="s">
         <v>324</v>
       </c>
-      <c r="C244" t="s">
-        <v>325</v>
-      </c>
       <c r="D244" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H244" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B245" t="s">
+        <v>325</v>
+      </c>
+      <c r="C245" t="s">
         <v>326</v>
       </c>
-      <c r="C245" t="s">
-        <v>327</v>
-      </c>
       <c r="D245" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H245" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B246" t="s">
+        <v>327</v>
+      </c>
+      <c r="C246" t="s">
         <v>328</v>
       </c>
-      <c r="C246" t="s">
-        <v>329</v>
-      </c>
       <c r="D246" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H246" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B247" t="s">
+        <v>329</v>
+      </c>
+      <c r="C247" t="s">
         <v>330</v>
       </c>
-      <c r="C247" t="s">
-        <v>331</v>
-      </c>
       <c r="D247" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H247" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B248" t="s">
+        <v>331</v>
+      </c>
+      <c r="C248" t="s">
         <v>332</v>
       </c>
-      <c r="C248" t="s">
-        <v>333</v>
-      </c>
       <c r="D248" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H248" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B249" t="s">
+        <v>333</v>
+      </c>
+      <c r="C249" t="s">
         <v>334</v>
       </c>
-      <c r="C249" t="s">
-        <v>335</v>
-      </c>
       <c r="D249" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H249" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B250" t="s">
+        <v>335</v>
+      </c>
+      <c r="C250" t="s">
         <v>336</v>
       </c>
-      <c r="C250" t="s">
-        <v>337</v>
-      </c>
       <c r="D250" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H250" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B251" t="s">
+        <v>337</v>
+      </c>
+      <c r="C251" t="s">
         <v>338</v>
       </c>
-      <c r="C251" t="s">
-        <v>339</v>
-      </c>
       <c r="D251" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H251" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B252" t="s">
+        <v>339</v>
+      </c>
+      <c r="C252" t="s">
         <v>340</v>
       </c>
-      <c r="C252" t="s">
-        <v>341</v>
-      </c>
       <c r="D252" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H252" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B253" t="s">
+        <v>341</v>
+      </c>
+      <c r="C253" t="s">
         <v>342</v>
       </c>
-      <c r="C253" t="s">
-        <v>343</v>
-      </c>
       <c r="D253" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H253" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B254" t="s">
+        <v>343</v>
+      </c>
+      <c r="C254" t="s">
         <v>344</v>
       </c>
-      <c r="C254" t="s">
-        <v>345</v>
-      </c>
       <c r="D254" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H254" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B255" t="s">
+        <v>345</v>
+      </c>
+      <c r="C255" t="s">
         <v>346</v>
       </c>
-      <c r="C255" t="s">
-        <v>347</v>
-      </c>
       <c r="D255" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H255" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B256" t="s">
+        <v>347</v>
+      </c>
+      <c r="C256" t="s">
         <v>348</v>
       </c>
-      <c r="C256" t="s">
-        <v>349</v>
-      </c>
       <c r="D256" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H256" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B257" t="s">
+        <v>349</v>
+      </c>
+      <c r="C257" t="s">
         <v>350</v>
       </c>
-      <c r="C257" t="s">
-        <v>351</v>
-      </c>
       <c r="D257" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H257" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B258" t="s">
+        <v>351</v>
+      </c>
+      <c r="C258" t="s">
         <v>352</v>
       </c>
-      <c r="C258" t="s">
-        <v>353</v>
-      </c>
       <c r="D258" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H258" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B259" t="s">
+        <v>353</v>
+      </c>
+      <c r="C259" t="s">
         <v>354</v>
       </c>
-      <c r="C259" t="s">
-        <v>355</v>
-      </c>
       <c r="D259" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H259" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B260" t="s">
+        <v>355</v>
+      </c>
+      <c r="C260" t="s">
         <v>356</v>
       </c>
-      <c r="C260" t="s">
-        <v>357</v>
-      </c>
       <c r="D260" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H260" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
+        <v>358</v>
+      </c>
+      <c r="B261" t="s">
         <v>359</v>
       </c>
-      <c r="B261" t="s">
-        <v>360</v>
-      </c>
       <c r="C261" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D261" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H261" t="s">
         <v>81</v>
@@ -6839,16 +6845,16 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B262" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C262" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D262" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H262" t="s">
         <v>81</v>
@@ -6856,16 +6862,16 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B263" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C263" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D263" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H263" t="s">
         <v>81</v>
@@ -6873,16 +6879,16 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B264" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C264" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D264" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H264" t="s">
         <v>81</v>
@@ -6890,16 +6896,16 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
+        <v>363</v>
+      </c>
+      <c r="B265" t="s">
         <v>364</v>
       </c>
-      <c r="B265" t="s">
-        <v>365</v>
-      </c>
       <c r="C265" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D265" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H265" t="s">
         <v>81</v>
@@ -6907,16 +6913,16 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B266" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C266" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D266" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H266" t="s">
         <v>81</v>
@@ -6924,16 +6930,16 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B267" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C267" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D267" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H267" t="s">
         <v>81</v>
@@ -6941,16 +6947,16 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B268" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C268" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D268" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H268" t="s">
         <v>81</v>
@@ -6958,16 +6964,16 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B269" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C269" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D269" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H269" t="s">
         <v>81</v>
@@ -6975,16 +6981,16 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B270" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C270" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D270" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H270" t="s">
         <v>81</v>
@@ -6995,13 +7001,13 @@
         <v>34</v>
       </c>
       <c r="B271" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C271" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D271" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H271" t="s">
         <v>81</v>
@@ -7012,13 +7018,13 @@
         <v>34</v>
       </c>
       <c r="B272" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C272" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D272" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H272" t="s">
         <v>81</v>
@@ -7029,13 +7035,13 @@
         <v>34</v>
       </c>
       <c r="B273" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C273" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D273" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H273" t="s">
         <v>81</v>
@@ -7043,16 +7049,16 @@
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B274" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="B274" s="3" t="s">
-        <v>373</v>
-      </c>
       <c r="C274" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D274" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H274" t="s">
         <v>81</v>
@@ -7060,16 +7066,16 @@
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D275" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H275" t="s">
         <v>81</v>
@@ -7077,16 +7083,16 @@
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D276" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H276" t="s">
         <v>81</v>
@@ -7094,16 +7100,16 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B277" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D277" t="s">
         <v>376</v>
-      </c>
-      <c r="C277" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="D277" t="s">
-        <v>377</v>
       </c>
       <c r="H277" t="s">
         <v>81</v>
@@ -7111,7 +7117,7 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B278" s="3" t="s">
         <v>37</v>
@@ -7120,7 +7126,7 @@
         <v>37</v>
       </c>
       <c r="D278" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H278" t="s">
         <v>81</v>
@@ -7128,54 +7134,30 @@
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>39</v>
+        <v>466</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D279" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H279" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A280" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C280" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D280" t="s">
-        <v>377</v>
-      </c>
-      <c r="H280" t="s">
-        <v>81</v>
-      </c>
+      <c r="A280" s="3"/>
+      <c r="B280" s="3"/>
+      <c r="C280" s="3"/>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A281" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C281" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D281" t="s">
-        <v>377</v>
-      </c>
-      <c r="H281" t="s">
-        <v>81</v>
-      </c>
+      <c r="A281" s="3"/>
+      <c r="B281" s="3"/>
+      <c r="C281" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated add_metrics with connection to db
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C336D64-9D00-4DA9-B583-C1BE6B5689FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157A9306-F09B-4F60-8C0A-8B95A4EACC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="16080" windowWidth="28110" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
@@ -2197,7 +2197,7 @@
   <dimension ref="A1:H281"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated interaction between database and selected files from data collection tab
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157A9306-F09B-4F60-8C0A-8B95A4EACC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC5008D-6B94-4090-ABBC-F2616C7FEB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="16080" windowWidth="28110" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="468">
   <si>
     <t>category</t>
   </si>
@@ -1760,12 +1760,6 @@
     <t>What is the number of employees that has the skills to perform maintenance tasks on hardware?</t>
   </si>
   <si>
-    <t>number of schools reached (number of projects)</t>
-  </si>
-  <si>
-    <t>number of students reached</t>
-  </si>
-  <si>
     <t>What is the number of employees (both staff and teachers) that has ICT literacy skills?</t>
   </si>
   <si>
@@ -1815,6 +1809,9 @@
   </si>
   <si>
     <t>New skills 2</t>
+  </si>
+  <si>
+    <t>Number of schools reached (number of projects)</t>
   </si>
 </sst>
 </file>
@@ -2196,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="B109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,13 +2222,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>390</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -2585,7 +2582,7 @@
         <v>419</v>
       </c>
       <c r="C22" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D22" t="s">
         <v>376</v>
@@ -2701,7 +2698,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C29" t="s">
         <v>443</v>
@@ -2925,7 +2922,7 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D42" t="s">
         <v>386</v>
@@ -2948,7 +2945,7 @@
         <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D43" t="s">
         <v>386</v>
@@ -3378,7 +3375,7 @@
         <v>5</v>
       </c>
       <c r="G66" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H66" t="s">
         <v>245</v>
@@ -3478,7 +3475,7 @@
         <v>389</v>
       </c>
       <c r="G71" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H71" t="s">
         <v>245</v>
@@ -3492,7 +3489,7 @@
         <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D72" t="s">
         <v>386</v>
@@ -3501,7 +3498,7 @@
         <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H72" t="s">
         <v>245</v>
@@ -3515,7 +3512,7 @@
         <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D73" t="s">
         <v>386</v>
@@ -3538,7 +3535,7 @@
         <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D74" t="s">
         <v>386</v>
@@ -3547,7 +3544,7 @@
         <v>4</v>
       </c>
       <c r="G74" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H74" t="s">
         <v>245</v>
@@ -3630,7 +3627,7 @@
         <v>389</v>
       </c>
       <c r="G78" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H78" t="s">
         <v>245</v>
@@ -3690,7 +3687,7 @@
         <v>389</v>
       </c>
       <c r="G81" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H81" t="s">
         <v>245</v>
@@ -4721,7 +4718,7 @@
         <v>229</v>
       </c>
       <c r="B142" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C142" t="s">
         <v>238</v>
@@ -4738,10 +4735,10 @@
         <v>229</v>
       </c>
       <c r="B143" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C143" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D143" t="s">
         <v>386</v>
@@ -4750,7 +4747,7 @@
         <v>3</v>
       </c>
       <c r="G143" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H143" t="s">
         <v>245</v>
@@ -4926,7 +4923,13 @@
         <v>97</v>
       </c>
       <c r="D153" t="s">
-        <v>60</v>
+        <v>386</v>
+      </c>
+      <c r="E153" s="5">
+        <v>7</v>
+      </c>
+      <c r="G153" t="s">
+        <v>391</v>
       </c>
       <c r="H153" t="s">
         <v>357</v>
@@ -5046,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="G159" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H159" t="s">
         <v>357</v>
@@ -5146,7 +5149,7 @@
         <v>389</v>
       </c>
       <c r="G164" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H164" t="s">
         <v>357</v>
@@ -5169,7 +5172,7 @@
         <v>5</v>
       </c>
       <c r="G165" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H165" t="s">
         <v>357</v>
@@ -5206,7 +5209,7 @@
         <v>114</v>
       </c>
       <c r="C167" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D167" t="s">
         <v>386</v>
@@ -5215,7 +5218,7 @@
         <v>4</v>
       </c>
       <c r="G167" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H167" t="s">
         <v>357</v>
@@ -5298,7 +5301,7 @@
         <v>389</v>
       </c>
       <c r="G171" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H171" t="s">
         <v>357</v>
@@ -5358,7 +5361,7 @@
         <v>389</v>
       </c>
       <c r="G174" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H174" t="s">
         <v>357</v>
@@ -7004,7 +7007,7 @@
         <v>432</v>
       </c>
       <c r="C271" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="D271" t="s">
         <v>376</v>
@@ -7021,7 +7024,7 @@
         <v>433</v>
       </c>
       <c r="C272" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="D272" t="s">
         <v>376</v>
@@ -7137,7 +7140,7 @@
         <v>363</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
added calculations for table
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC5008D-6B94-4090-ABBC-F2616C7FEB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD5276D-FA9D-41C6-9F73-6F519BDD37C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="473">
   <si>
     <t>category</t>
   </si>
@@ -1812,6 +1812,21 @@
   </si>
   <si>
     <t>Number of schools reached (number of projects)</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -2191,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
-  <dimension ref="A1:H281"/>
+  <dimension ref="A1:I281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,9 +2221,10 @@
     <col min="5" max="5" width="11.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.75" style="5" customWidth="1"/>
     <col min="7" max="7" width="21.75" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2233,8 +2249,11 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2250,8 +2269,11 @@
       <c r="H2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2267,8 +2289,11 @@
       <c r="H3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2284,8 +2309,11 @@
       <c r="H4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2301,8 +2329,11 @@
       <c r="H5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2318,8 +2349,11 @@
       <c r="H6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2335,8 +2369,11 @@
       <c r="H7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2352,8 +2389,11 @@
       <c r="H8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2369,8 +2409,11 @@
       <c r="H9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2386,8 +2429,11 @@
       <c r="H10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2403,8 +2449,11 @@
       <c r="H11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2420,8 +2469,11 @@
       <c r="H12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2437,8 +2489,11 @@
       <c r="H13" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2454,8 +2509,11 @@
       <c r="H14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2471,8 +2529,11 @@
       <c r="H15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2488,8 +2549,11 @@
       <c r="H16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2505,8 +2569,11 @@
       <c r="H17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2522,8 +2589,11 @@
       <c r="H18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2539,8 +2609,11 @@
       <c r="H19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2556,8 +2629,11 @@
       <c r="H20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2573,8 +2649,11 @@
       <c r="H21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2590,8 +2669,11 @@
       <c r="H22" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2607,8 +2689,11 @@
       <c r="H23" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2624,8 +2709,11 @@
       <c r="H24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2641,8 +2729,11 @@
       <c r="H25" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2658,8 +2749,11 @@
       <c r="H26" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2675,8 +2769,11 @@
       <c r="H27" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2692,8 +2789,11 @@
       <c r="H28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2709,8 +2809,11 @@
       <c r="H29" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2726,8 +2829,11 @@
       <c r="H30" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -2743,8 +2849,11 @@
       <c r="H31" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2760,8 +2869,11 @@
       <c r="H32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2777,8 +2889,11 @@
       <c r="H33" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2794,8 +2909,11 @@
       <c r="H34" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2811,8 +2929,11 @@
       <c r="H35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2828,8 +2949,11 @@
       <c r="H36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -2845,8 +2969,11 @@
       <c r="H37" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2862,8 +2989,11 @@
       <c r="H38" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2879,8 +3009,11 @@
       <c r="H39" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2896,8 +3029,11 @@
       <c r="H40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2913,8 +3049,11 @@
       <c r="H41" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2936,8 +3075,11 @@
       <c r="H42" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2959,8 +3101,11 @@
       <c r="H43" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -2976,8 +3121,11 @@
       <c r="H44" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -2993,8 +3141,11 @@
       <c r="H45" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -3010,8 +3161,11 @@
       <c r="H46" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -3027,8 +3181,11 @@
       <c r="H47" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -3044,8 +3201,11 @@
       <c r="H48" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -3061,8 +3221,11 @@
       <c r="H49" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -3078,8 +3241,11 @@
       <c r="H50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -3095,8 +3261,11 @@
       <c r="H51" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -3112,8 +3281,11 @@
       <c r="H52" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -3129,8 +3301,11 @@
       <c r="H53" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -3146,8 +3321,11 @@
       <c r="H54" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -3169,8 +3347,11 @@
       <c r="H55" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -3186,8 +3367,11 @@
       <c r="H56" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -3203,8 +3387,11 @@
       <c r="H57" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -3220,8 +3407,11 @@
       <c r="H58" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3237,8 +3427,11 @@
       <c r="H59" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -3260,8 +3453,11 @@
       <c r="H60" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3277,8 +3473,11 @@
       <c r="H61" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -3294,8 +3493,11 @@
       <c r="H62" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -3317,8 +3519,11 @@
       <c r="H63" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>98</v>
       </c>
@@ -3340,8 +3545,11 @@
       <c r="H64" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -3357,8 +3565,11 @@
       <c r="H65" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -3380,8 +3591,11 @@
       <c r="H66" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -3397,8 +3611,11 @@
       <c r="H67" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -3414,8 +3631,11 @@
       <c r="H68" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>62</v>
       </c>
@@ -3431,8 +3651,11 @@
       <c r="H69" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>62</v>
       </c>
@@ -3454,8 +3677,11 @@
       <c r="H70" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -3480,8 +3706,11 @@
       <c r="H71" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -3503,8 +3732,11 @@
       <c r="H72" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3526,8 +3758,11 @@
       <c r="H73" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -3549,8 +3784,11 @@
       <c r="H74" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -3572,8 +3810,11 @@
       <c r="H75" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>116</v>
       </c>
@@ -3589,8 +3830,11 @@
       <c r="H76" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>116</v>
       </c>
@@ -3606,8 +3850,11 @@
       <c r="H77" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>116</v>
       </c>
@@ -3632,8 +3879,11 @@
       <c r="H78" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>122</v>
       </c>
@@ -3649,8 +3899,11 @@
       <c r="H79" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>122</v>
       </c>
@@ -3666,8 +3919,11 @@
       <c r="H80" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>122</v>
       </c>
@@ -3692,8 +3948,11 @@
       <c r="H81" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -3709,8 +3968,11 @@
       <c r="H82" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -3726,8 +3988,11 @@
       <c r="H83" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -3743,8 +4008,11 @@
       <c r="H84" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3760,8 +4028,11 @@
       <c r="H85" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>96</v>
       </c>
@@ -3777,8 +4048,11 @@
       <c r="H86" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -3794,8 +4068,11 @@
       <c r="H87" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>137</v>
       </c>
@@ -3811,8 +4088,11 @@
       <c r="H88" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>137</v>
       </c>
@@ -3828,8 +4108,11 @@
       <c r="H89" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -3845,8 +4128,11 @@
       <c r="H90" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -3862,8 +4148,11 @@
       <c r="H91" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -3879,8 +4168,11 @@
       <c r="H92" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -3896,8 +4188,11 @@
       <c r="H93" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -3913,8 +4208,11 @@
       <c r="H94" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -3930,8 +4228,11 @@
       <c r="H95" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>58</v>
       </c>
@@ -3947,8 +4248,11 @@
       <c r="H96" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -3964,8 +4268,11 @@
       <c r="H97" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>58</v>
       </c>
@@ -3981,8 +4288,11 @@
       <c r="H98" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>62</v>
       </c>
@@ -3998,8 +4308,11 @@
       <c r="H99" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>62</v>
       </c>
@@ -4015,8 +4328,11 @@
       <c r="H100" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>62</v>
       </c>
@@ -4032,8 +4348,11 @@
       <c r="H101" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>62</v>
       </c>
@@ -4049,8 +4368,11 @@
       <c r="H102" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>166</v>
       </c>
@@ -4066,8 +4388,11 @@
       <c r="H103" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>166</v>
       </c>
@@ -4083,8 +4408,11 @@
       <c r="H104" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>166</v>
       </c>
@@ -4100,8 +4428,11 @@
       <c r="H105" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>166</v>
       </c>
@@ -4117,8 +4448,11 @@
       <c r="H106" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>166</v>
       </c>
@@ -4134,8 +4468,11 @@
       <c r="H107" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>166</v>
       </c>
@@ -4151,8 +4488,11 @@
       <c r="H108" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -4168,8 +4508,11 @@
       <c r="H109" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4185,8 +4528,11 @@
       <c r="H110" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>122</v>
       </c>
@@ -4202,8 +4548,11 @@
       <c r="H111" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>122</v>
       </c>
@@ -4219,8 +4568,11 @@
       <c r="H112" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>187</v>
       </c>
@@ -4236,8 +4588,11 @@
       <c r="H113" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>187</v>
       </c>
@@ -4253,8 +4608,11 @@
       <c r="H114" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>187</v>
       </c>
@@ -4270,8 +4628,11 @@
       <c r="H115" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>187</v>
       </c>
@@ -4287,8 +4648,11 @@
       <c r="H116" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>187</v>
       </c>
@@ -4304,8 +4668,11 @@
       <c r="H117" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>187</v>
       </c>
@@ -4321,8 +4688,11 @@
       <c r="H118" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>200</v>
       </c>
@@ -4338,8 +4708,11 @@
       <c r="H119" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>200</v>
       </c>
@@ -4355,8 +4728,11 @@
       <c r="H120" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>200</v>
       </c>
@@ -4372,8 +4748,11 @@
       <c r="H121" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -4389,8 +4768,11 @@
       <c r="H122" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>200</v>
       </c>
@@ -4406,8 +4788,11 @@
       <c r="H123" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>200</v>
       </c>
@@ -4423,8 +4808,11 @@
       <c r="H124" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>207</v>
       </c>
@@ -4440,8 +4828,11 @@
       <c r="H125" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>207</v>
       </c>
@@ -4457,8 +4848,11 @@
       <c r="H126" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>207</v>
       </c>
@@ -4474,8 +4868,11 @@
       <c r="H127" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>207</v>
       </c>
@@ -4491,8 +4888,11 @@
       <c r="H128" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>207</v>
       </c>
@@ -4508,8 +4908,11 @@
       <c r="H129" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>207</v>
       </c>
@@ -4525,8 +4928,11 @@
       <c r="H130" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -4542,8 +4948,11 @@
       <c r="H131" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>96</v>
       </c>
@@ -4559,8 +4968,11 @@
       <c r="H132" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>218</v>
       </c>
@@ -4576,8 +4988,11 @@
       <c r="H133" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>218</v>
       </c>
@@ -4593,8 +5008,11 @@
       <c r="H134" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>218</v>
       </c>
@@ -4610,8 +5028,11 @@
       <c r="H135" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>218</v>
       </c>
@@ -4627,8 +5048,11 @@
       <c r="H136" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>218</v>
       </c>
@@ -4644,8 +5068,11 @@
       <c r="H137" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>229</v>
       </c>
@@ -4661,8 +5088,11 @@
       <c r="H138" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>229</v>
       </c>
@@ -4678,8 +5108,11 @@
       <c r="H139" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>229</v>
       </c>
@@ -4695,8 +5128,11 @@
       <c r="H140" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>229</v>
       </c>
@@ -4712,8 +5148,11 @@
       <c r="H141" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>229</v>
       </c>
@@ -4729,8 +5168,11 @@
       <c r="H142" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -4752,8 +5194,11 @@
       <c r="H143" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>229</v>
       </c>
@@ -4769,8 +5214,11 @@
       <c r="H144" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>229</v>
       </c>
@@ -4786,8 +5234,11 @@
       <c r="H145" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>229</v>
       </c>
@@ -4803,8 +5254,11 @@
       <c r="H146" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>82</v>
       </c>
@@ -4820,8 +5274,11 @@
       <c r="H147" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>82</v>
       </c>
@@ -4843,8 +5300,11 @@
       <c r="H148" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>82</v>
       </c>
@@ -4860,8 +5320,11 @@
       <c r="H149" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>82</v>
       </c>
@@ -4877,8 +5340,11 @@
       <c r="H150" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>82</v>
       </c>
@@ -4894,8 +5360,11 @@
       <c r="H151" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>82</v>
       </c>
@@ -4911,8 +5380,11 @@
       <c r="H152" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>82</v>
       </c>
@@ -4934,8 +5406,11 @@
       <c r="H153" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>82</v>
       </c>
@@ -4951,8 +5426,11 @@
       <c r="H154" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>82</v>
       </c>
@@ -4968,8 +5446,11 @@
       <c r="H155" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>98</v>
       </c>
@@ -4991,8 +5472,11 @@
       <c r="H156" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>98</v>
       </c>
@@ -5014,8 +5498,11 @@
       <c r="H157" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>101</v>
       </c>
@@ -5031,8 +5518,11 @@
       <c r="H158" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>101</v>
       </c>
@@ -5043,7 +5533,7 @@
         <v>402</v>
       </c>
       <c r="D159" t="s">
-        <v>386</v>
+        <v>60</v>
       </c>
       <c r="E159" s="5">
         <v>5</v>
@@ -5054,8 +5544,11 @@
       <c r="H159" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>58</v>
       </c>
@@ -5071,8 +5564,11 @@
       <c r="H160" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>62</v>
       </c>
@@ -5088,8 +5584,11 @@
       <c r="H161" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>62</v>
       </c>
@@ -5105,8 +5604,11 @@
       <c r="H162" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>62</v>
       </c>
@@ -5128,8 +5630,11 @@
       <c r="H163" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>62</v>
       </c>
@@ -5154,8 +5659,11 @@
       <c r="H164" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>79</v>
       </c>
@@ -5177,8 +5685,11 @@
       <c r="H165" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>79</v>
       </c>
@@ -5200,8 +5711,11 @@
       <c r="H166" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>79</v>
       </c>
@@ -5223,8 +5737,11 @@
       <c r="H167" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>79</v>
       </c>
@@ -5246,8 +5763,11 @@
       <c r="H168" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>116</v>
       </c>
@@ -5263,8 +5783,11 @@
       <c r="H169" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>116</v>
       </c>
@@ -5280,8 +5803,11 @@
       <c r="H170" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>116</v>
       </c>
@@ -5306,8 +5832,11 @@
       <c r="H171" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>122</v>
       </c>
@@ -5323,8 +5852,11 @@
       <c r="H172" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>122</v>
       </c>
@@ -5340,8 +5872,11 @@
       <c r="H173" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>122</v>
       </c>
@@ -5366,8 +5901,11 @@
       <c r="H174" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>14</v>
       </c>
@@ -5383,8 +5921,11 @@
       <c r="H175" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>14</v>
       </c>
@@ -5400,8 +5941,11 @@
       <c r="H176" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>96</v>
       </c>
@@ -5417,8 +5961,11 @@
       <c r="H177" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>137</v>
       </c>
@@ -5434,8 +5981,11 @@
       <c r="H178" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>137</v>
       </c>
@@ -5451,8 +6001,11 @@
       <c r="H179" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>137</v>
       </c>
@@ -5468,8 +6021,11 @@
       <c r="H180" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>137</v>
       </c>
@@ -5485,8 +6041,11 @@
       <c r="H181" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>137</v>
       </c>
@@ -5502,8 +6061,11 @@
       <c r="H182" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>98</v>
       </c>
@@ -5519,8 +6081,11 @@
       <c r="H183" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>98</v>
       </c>
@@ -5536,8 +6101,11 @@
       <c r="H184" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>101</v>
       </c>
@@ -5553,8 +6121,11 @@
       <c r="H185" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>101</v>
       </c>
@@ -5570,8 +6141,11 @@
       <c r="H186" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>101</v>
       </c>
@@ -5587,8 +6161,11 @@
       <c r="H187" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>58</v>
       </c>
@@ -5604,8 +6181,11 @@
       <c r="H188" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>58</v>
       </c>
@@ -5621,8 +6201,11 @@
       <c r="H189" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>58</v>
       </c>
@@ -5638,8 +6221,11 @@
       <c r="H190" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>58</v>
       </c>
@@ -5655,8 +6241,11 @@
       <c r="H191" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>62</v>
       </c>
@@ -5672,8 +6261,11 @@
       <c r="H192" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>62</v>
       </c>
@@ -5689,8 +6281,11 @@
       <c r="H193" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>62</v>
       </c>
@@ -5706,8 +6301,11 @@
       <c r="H194" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I194" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>62</v>
       </c>
@@ -5723,8 +6321,11 @@
       <c r="H195" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I195" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>116</v>
       </c>
@@ -5740,8 +6341,11 @@
       <c r="H196" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I196" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>116</v>
       </c>
@@ -5757,8 +6361,11 @@
       <c r="H197" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I197" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>122</v>
       </c>
@@ -5774,8 +6381,11 @@
       <c r="H198" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I198" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>122</v>
       </c>
@@ -5791,8 +6401,11 @@
       <c r="H199" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I199" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>271</v>
       </c>
@@ -5808,8 +6421,11 @@
       <c r="H200" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I200" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>271</v>
       </c>
@@ -5825,8 +6441,11 @@
       <c r="H201" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I201" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>271</v>
       </c>
@@ -5842,8 +6461,11 @@
       <c r="H202" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>271</v>
       </c>
@@ -5859,8 +6481,11 @@
       <c r="H203" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I203" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>271</v>
       </c>
@@ -5876,8 +6501,11 @@
       <c r="H204" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I204" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>271</v>
       </c>
@@ -5893,8 +6521,11 @@
       <c r="H205" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I205" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>271</v>
       </c>
@@ -5910,8 +6541,11 @@
       <c r="H206" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I206" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>271</v>
       </c>
@@ -5927,8 +6561,11 @@
       <c r="H207" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>271</v>
       </c>
@@ -5944,8 +6581,11 @@
       <c r="H208" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I208" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>271</v>
       </c>
@@ -5961,8 +6601,11 @@
       <c r="H209" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I209" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>271</v>
       </c>
@@ -5978,8 +6621,11 @@
       <c r="H210" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I210" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>271</v>
       </c>
@@ -5995,8 +6641,11 @@
       <c r="H211" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I211" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>187</v>
       </c>
@@ -6012,8 +6661,11 @@
       <c r="H212" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I212" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>187</v>
       </c>
@@ -6029,8 +6681,11 @@
       <c r="H213" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I213" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>187</v>
       </c>
@@ -6046,8 +6701,11 @@
       <c r="H214" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I214" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>187</v>
       </c>
@@ -6063,8 +6721,11 @@
       <c r="H215" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I215" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>187</v>
       </c>
@@ -6080,8 +6741,11 @@
       <c r="H216" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I216" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>187</v>
       </c>
@@ -6097,8 +6761,11 @@
       <c r="H217" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I217" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>200</v>
       </c>
@@ -6114,8 +6781,11 @@
       <c r="H218" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I218" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>200</v>
       </c>
@@ -6131,8 +6801,11 @@
       <c r="H219" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I219" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>200</v>
       </c>
@@ -6148,8 +6821,11 @@
       <c r="H220" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I220" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>200</v>
       </c>
@@ -6165,8 +6841,11 @@
       <c r="H221" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I221" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>200</v>
       </c>
@@ -6182,8 +6861,11 @@
       <c r="H222" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I222" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>200</v>
       </c>
@@ -6199,8 +6881,11 @@
       <c r="H223" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I223" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>207</v>
       </c>
@@ -6216,8 +6901,11 @@
       <c r="H224" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I224" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>207</v>
       </c>
@@ -6233,8 +6921,11 @@
       <c r="H225" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I225" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>207</v>
       </c>
@@ -6250,8 +6941,11 @@
       <c r="H226" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I226" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>207</v>
       </c>
@@ -6267,8 +6961,11 @@
       <c r="H227" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I227" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>207</v>
       </c>
@@ -6284,8 +6981,11 @@
       <c r="H228" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I228" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>207</v>
       </c>
@@ -6301,8 +7001,11 @@
       <c r="H229" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I229" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>294</v>
       </c>
@@ -6318,8 +7021,11 @@
       <c r="H230" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I230" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>294</v>
       </c>
@@ -6335,8 +7041,11 @@
       <c r="H231" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I231" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>294</v>
       </c>
@@ -6352,8 +7061,11 @@
       <c r="H232" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I232" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>294</v>
       </c>
@@ -6369,8 +7081,11 @@
       <c r="H233" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I233" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>294</v>
       </c>
@@ -6386,8 +7101,11 @@
       <c r="H234" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I234" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>294</v>
       </c>
@@ -6403,8 +7121,11 @@
       <c r="H235" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I235" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>294</v>
       </c>
@@ -6420,8 +7141,11 @@
       <c r="H236" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I236" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>294</v>
       </c>
@@ -6437,8 +7161,11 @@
       <c r="H237" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I237" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>294</v>
       </c>
@@ -6454,8 +7181,11 @@
       <c r="H238" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I238" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>294</v>
       </c>
@@ -6471,8 +7201,11 @@
       <c r="H239" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I239" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>294</v>
       </c>
@@ -6488,8 +7221,11 @@
       <c r="H240" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I240" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>294</v>
       </c>
@@ -6505,8 +7241,11 @@
       <c r="H241" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I241" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>294</v>
       </c>
@@ -6522,8 +7261,11 @@
       <c r="H242" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I242" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>294</v>
       </c>
@@ -6539,8 +7281,11 @@
       <c r="H243" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I243" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>294</v>
       </c>
@@ -6556,8 +7301,11 @@
       <c r="H244" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I244" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>294</v>
       </c>
@@ -6573,8 +7321,11 @@
       <c r="H245" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I245" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>294</v>
       </c>
@@ -6590,8 +7341,11 @@
       <c r="H246" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I246" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>294</v>
       </c>
@@ -6607,8 +7361,11 @@
       <c r="H247" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I247" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>294</v>
       </c>
@@ -6624,8 +7381,11 @@
       <c r="H248" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I248" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>294</v>
       </c>
@@ -6641,8 +7401,11 @@
       <c r="H249" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I249" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>294</v>
       </c>
@@ -6658,8 +7421,11 @@
       <c r="H250" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I250" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>294</v>
       </c>
@@ -6675,8 +7441,11 @@
       <c r="H251" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I251" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>294</v>
       </c>
@@ -6692,8 +7461,11 @@
       <c r="H252" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I252" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>294</v>
       </c>
@@ -6709,8 +7481,11 @@
       <c r="H253" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I253" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>294</v>
       </c>
@@ -6726,8 +7501,11 @@
       <c r="H254" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I254" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>294</v>
       </c>
@@ -6743,8 +7521,11 @@
       <c r="H255" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I255" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>294</v>
       </c>
@@ -6760,8 +7541,11 @@
       <c r="H256" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I256" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>294</v>
       </c>
@@ -6777,8 +7561,11 @@
       <c r="H257" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I257" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>294</v>
       </c>
@@ -6794,8 +7581,11 @@
       <c r="H258" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I258" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>294</v>
       </c>
@@ -6811,8 +7601,11 @@
       <c r="H259" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I259" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>294</v>
       </c>
@@ -6828,8 +7621,11 @@
       <c r="H260" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I260" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>358</v>
       </c>
@@ -6845,8 +7641,11 @@
       <c r="H261" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I261" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>358</v>
       </c>
@@ -6862,8 +7661,11 @@
       <c r="H262" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I262" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>358</v>
       </c>
@@ -6879,8 +7681,11 @@
       <c r="H263" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I263" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>358</v>
       </c>
@@ -6896,8 +7701,11 @@
       <c r="H264" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I264" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>363</v>
       </c>
@@ -6913,8 +7721,11 @@
       <c r="H265" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I265" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>363</v>
       </c>
@@ -6930,8 +7741,11 @@
       <c r="H266" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I266" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>363</v>
       </c>
@@ -6947,8 +7761,11 @@
       <c r="H267" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I267" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>363</v>
       </c>
@@ -6964,8 +7781,11 @@
       <c r="H268" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I268" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>363</v>
       </c>
@@ -6981,8 +7801,11 @@
       <c r="H269" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I269" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>363</v>
       </c>
@@ -6998,8 +7821,11 @@
       <c r="H270" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I270" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>34</v>
       </c>
@@ -7015,8 +7841,11 @@
       <c r="H271" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I271" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>34</v>
       </c>
@@ -7032,8 +7861,11 @@
       <c r="H272" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I272" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>34</v>
       </c>
@@ -7049,8 +7881,11 @@
       <c r="H273" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I273" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>371</v>
       </c>
@@ -7066,8 +7901,11 @@
       <c r="H274" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I274" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>371</v>
       </c>
@@ -7083,8 +7921,11 @@
       <c r="H275" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I275" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>371</v>
       </c>
@@ -7100,8 +7941,11 @@
       <c r="H276" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I276" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>371</v>
       </c>
@@ -7117,8 +7961,11 @@
       <c r="H277" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I277" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>363</v>
       </c>
@@ -7134,8 +7981,11 @@
       <c r="H278" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I278" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>363</v>
       </c>
@@ -7151,13 +8001,16 @@
       <c r="H279" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I279" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="3"/>
       <c r="B280" s="3"/>
       <c r="C280" s="3"/>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="3"/>
       <c r="B281" s="3"/>
       <c r="C281" s="3"/>

</xml_diff>

<commit_message>
fixed table selection from uploaded files
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FEFF6B-E571-4F2F-9942-416FE49E9AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39195AE2-DB31-4B14-B762-9FC5E5975C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
@@ -1736,9 +1736,6 @@
     <t>What is the number of teachers that left your school in the past year?</t>
   </si>
   <si>
-    <t>What is the number of students that repeats current year in your school/project environment?</t>
-  </si>
-  <si>
     <t>What is the number of Personal Computers that is available within the school/project environment (for both staff and students)?</t>
   </si>
   <si>
@@ -1827,6 +1824,9 @@
   </si>
   <si>
     <t>Likert_7</t>
+  </si>
+  <si>
+    <t>What is the ratio of students that repeats current year in your school/project environment?</t>
   </si>
 </sst>
 </file>
@@ -2206,16 +2206,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
-  <dimension ref="A1:I281"/>
+  <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.25" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="67.625" customWidth="1"/>
     <col min="3" max="3" width="97.875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="5" customWidth="1"/>
@@ -2224,7 +2224,7 @@
     <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2238,22 +2238,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>389</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2270,10 +2271,10 @@
         <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2290,10 +2291,10 @@
         <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2310,10 +2311,10 @@
         <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2330,10 +2331,10 @@
         <v>80</v>
       </c>
       <c r="I5" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2350,10 +2351,10 @@
         <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2370,10 +2371,10 @@
         <v>80</v>
       </c>
       <c r="I7" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2390,10 +2391,10 @@
         <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2410,10 +2411,10 @@
         <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2430,10 +2431,10 @@
         <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2450,10 +2451,10 @@
         <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2470,10 +2471,10 @@
         <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2490,10 +2491,10 @@
         <v>80</v>
       </c>
       <c r="I13" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2510,10 +2511,10 @@
         <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2530,10 +2531,10 @@
         <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2570,7 +2571,7 @@
         <v>80</v>
       </c>
       <c r="I17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2590,7 +2591,7 @@
         <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2610,7 +2611,7 @@
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2630,7 +2631,7 @@
         <v>80</v>
       </c>
       <c r="I20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2650,7 +2651,7 @@
         <v>80</v>
       </c>
       <c r="I21" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2661,7 +2662,7 @@
         <v>418</v>
       </c>
       <c r="C22" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D22" t="s">
         <v>375</v>
@@ -2670,7 +2671,7 @@
         <v>80</v>
       </c>
       <c r="I22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2690,7 +2691,7 @@
         <v>80</v>
       </c>
       <c r="I23" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2710,7 +2711,7 @@
         <v>80</v>
       </c>
       <c r="I24" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2730,7 +2731,7 @@
         <v>80</v>
       </c>
       <c r="I25" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2750,7 +2751,7 @@
         <v>80</v>
       </c>
       <c r="I26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2770,7 +2771,7 @@
         <v>80</v>
       </c>
       <c r="I27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2790,7 +2791,7 @@
         <v>80</v>
       </c>
       <c r="I28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2798,10 +2799,10 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C29" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
       <c r="D29" t="s">
         <v>375</v>
@@ -2830,7 +2831,7 @@
         <v>80</v>
       </c>
       <c r="I30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2841,7 +2842,7 @@
         <v>424</v>
       </c>
       <c r="C31" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D31" t="s">
         <v>375</v>
@@ -2850,7 +2851,7 @@
         <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,7 +2862,7 @@
         <v>425</v>
       </c>
       <c r="C32" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D32" t="s">
         <v>375</v>
@@ -2870,7 +2871,7 @@
         <v>80</v>
       </c>
       <c r="I32" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,7 +2882,7 @@
         <v>426</v>
       </c>
       <c r="C33" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D33" t="s">
         <v>375</v>
@@ -2890,7 +2891,7 @@
         <v>80</v>
       </c>
       <c r="I33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2910,7 +2911,7 @@
         <v>80</v>
       </c>
       <c r="I34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2930,7 +2931,7 @@
         <v>80</v>
       </c>
       <c r="I35" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2950,7 +2951,7 @@
         <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2970,7 +2971,7 @@
         <v>80</v>
       </c>
       <c r="I37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2990,7 +2991,7 @@
         <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3001,7 +3002,7 @@
         <v>427</v>
       </c>
       <c r="C39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D39" t="s">
         <v>375</v>
@@ -3010,7 +3011,7 @@
         <v>80</v>
       </c>
       <c r="I39" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3030,7 +3031,7 @@
         <v>80</v>
       </c>
       <c r="I40" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3050,7 +3051,7 @@
         <v>80</v>
       </c>
       <c r="I41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3061,7 +3062,7 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D42" t="s">
         <v>385</v>
@@ -3076,7 +3077,7 @@
         <v>80</v>
       </c>
       <c r="I42" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3087,7 +3088,7 @@
         <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D43" t="s">
         <v>385</v>
@@ -3102,7 +3103,7 @@
         <v>80</v>
       </c>
       <c r="I43" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3113,7 +3114,7 @@
         <v>428</v>
       </c>
       <c r="C44" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D44" t="s">
         <v>375</v>
@@ -3122,7 +3123,7 @@
         <v>80</v>
       </c>
       <c r="I44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3142,7 +3143,7 @@
         <v>80</v>
       </c>
       <c r="I45" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3162,7 +3163,7 @@
         <v>80</v>
       </c>
       <c r="I46" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3182,7 +3183,7 @@
         <v>80</v>
       </c>
       <c r="I47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3202,7 +3203,7 @@
         <v>80</v>
       </c>
       <c r="I48" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3222,7 +3223,7 @@
         <v>80</v>
       </c>
       <c r="I49" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3242,7 +3243,7 @@
         <v>80</v>
       </c>
       <c r="I50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3262,7 +3263,7 @@
         <v>80</v>
       </c>
       <c r="I51" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3282,7 +3283,7 @@
         <v>80</v>
       </c>
       <c r="I52" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3293,7 +3294,7 @@
         <v>430</v>
       </c>
       <c r="C53" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D53" t="s">
         <v>375</v>
@@ -3302,7 +3303,7 @@
         <v>80</v>
       </c>
       <c r="I53" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3322,7 +3323,7 @@
         <v>244</v>
       </c>
       <c r="I54" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3348,7 +3349,7 @@
         <v>244</v>
       </c>
       <c r="I55" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3368,7 +3369,7 @@
         <v>244</v>
       </c>
       <c r="I56" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3388,7 +3389,7 @@
         <v>244</v>
       </c>
       <c r="I57" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3408,7 +3409,7 @@
         <v>244</v>
       </c>
       <c r="I58" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3428,7 +3429,7 @@
         <v>244</v>
       </c>
       <c r="I59" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3454,7 +3455,7 @@
         <v>244</v>
       </c>
       <c r="I60" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3474,7 +3475,7 @@
         <v>244</v>
       </c>
       <c r="I61" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3494,7 +3495,7 @@
         <v>244</v>
       </c>
       <c r="I62" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3520,7 +3521,7 @@
         <v>244</v>
       </c>
       <c r="I63" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3546,7 +3547,7 @@
         <v>244</v>
       </c>
       <c r="I64" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3566,7 +3567,7 @@
         <v>244</v>
       </c>
       <c r="I65" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3586,13 +3587,13 @@
         <v>5</v>
       </c>
       <c r="G66" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H66" t="s">
         <v>244</v>
       </c>
       <c r="I66" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3612,7 +3613,7 @@
         <v>244</v>
       </c>
       <c r="I67" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3632,7 +3633,7 @@
         <v>244</v>
       </c>
       <c r="I68" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3652,7 +3653,7 @@
         <v>244</v>
       </c>
       <c r="I69" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3678,7 +3679,7 @@
         <v>244</v>
       </c>
       <c r="I70" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3701,13 +3702,13 @@
         <v>388</v>
       </c>
       <c r="G71" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H71" t="s">
         <v>244</v>
       </c>
       <c r="I71" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3718,7 +3719,7 @@
         <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D72" t="s">
         <v>385</v>
@@ -3727,13 +3728,13 @@
         <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H72" t="s">
         <v>244</v>
       </c>
       <c r="I72" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3744,7 +3745,7 @@
         <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D73" t="s">
         <v>385</v>
@@ -3759,7 +3760,7 @@
         <v>244</v>
       </c>
       <c r="I73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3770,7 +3771,7 @@
         <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D74" t="s">
         <v>385</v>
@@ -3779,13 +3780,13 @@
         <v>4</v>
       </c>
       <c r="G74" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H74" t="s">
         <v>244</v>
       </c>
       <c r="I74" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3811,7 +3812,7 @@
         <v>244</v>
       </c>
       <c r="I75" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3831,7 +3832,7 @@
         <v>244</v>
       </c>
       <c r="I76" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3851,7 +3852,7 @@
         <v>244</v>
       </c>
       <c r="I77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3874,13 +3875,13 @@
         <v>388</v>
       </c>
       <c r="G78" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H78" t="s">
         <v>244</v>
       </c>
       <c r="I78" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3900,7 +3901,7 @@
         <v>244</v>
       </c>
       <c r="I79" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3920,7 +3921,7 @@
         <v>244</v>
       </c>
       <c r="I80" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3943,13 +3944,13 @@
         <v>388</v>
       </c>
       <c r="G81" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H81" t="s">
         <v>244</v>
       </c>
       <c r="I81" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3969,7 +3970,7 @@
         <v>244</v>
       </c>
       <c r="I82" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3989,7 +3990,7 @@
         <v>244</v>
       </c>
       <c r="I83" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4003,13 +4004,13 @@
         <v>129</v>
       </c>
       <c r="D84" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H84" t="s">
         <v>244</v>
       </c>
       <c r="I84" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4023,13 +4024,13 @@
         <v>131</v>
       </c>
       <c r="D85" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H85" t="s">
         <v>244</v>
       </c>
       <c r="I85" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4043,13 +4044,13 @@
         <v>133</v>
       </c>
       <c r="D86" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H86" t="s">
         <v>244</v>
       </c>
       <c r="I86" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4063,13 +4064,13 @@
         <v>135</v>
       </c>
       <c r="D87" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H87" t="s">
         <v>244</v>
       </c>
       <c r="I87" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -4083,13 +4084,13 @@
         <v>138</v>
       </c>
       <c r="D88" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H88" t="s">
         <v>244</v>
       </c>
       <c r="I88" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4103,13 +4104,13 @@
         <v>140</v>
       </c>
       <c r="D89" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H89" t="s">
         <v>244</v>
       </c>
       <c r="I89" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4123,13 +4124,13 @@
         <v>142</v>
       </c>
       <c r="D90" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H90" t="s">
         <v>244</v>
       </c>
       <c r="I90" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4143,13 +4144,13 @@
         <v>144</v>
       </c>
       <c r="D91" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H91" t="s">
         <v>244</v>
       </c>
       <c r="I91" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4163,13 +4164,13 @@
         <v>407</v>
       </c>
       <c r="D92" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H92" t="s">
         <v>244</v>
       </c>
       <c r="I92" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4183,13 +4184,13 @@
         <v>147</v>
       </c>
       <c r="D93" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H93" t="s">
         <v>244</v>
       </c>
       <c r="I93" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4203,13 +4204,13 @@
         <v>149</v>
       </c>
       <c r="D94" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H94" t="s">
         <v>244</v>
       </c>
       <c r="I94" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4223,13 +4224,13 @@
         <v>151</v>
       </c>
       <c r="D95" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H95" t="s">
         <v>244</v>
       </c>
       <c r="I95" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4243,13 +4244,13 @@
         <v>153</v>
       </c>
       <c r="D96" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H96" t="s">
         <v>244</v>
       </c>
       <c r="I96" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4263,13 +4264,13 @@
         <v>155</v>
       </c>
       <c r="D97" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H97" t="s">
         <v>244</v>
       </c>
       <c r="I97" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4283,13 +4284,13 @@
         <v>157</v>
       </c>
       <c r="D98" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H98" t="s">
         <v>244</v>
       </c>
       <c r="I98" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4303,13 +4304,13 @@
         <v>408</v>
       </c>
       <c r="D99" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H99" t="s">
         <v>244</v>
       </c>
       <c r="I99" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,13 +4324,13 @@
         <v>160</v>
       </c>
       <c r="D100" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H100" t="s">
         <v>244</v>
       </c>
       <c r="I100" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4343,13 +4344,13 @@
         <v>162</v>
       </c>
       <c r="D101" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H101" t="s">
         <v>244</v>
       </c>
       <c r="I101" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4363,13 +4364,13 @@
         <v>164</v>
       </c>
       <c r="D102" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H102" t="s">
         <v>244</v>
       </c>
       <c r="I102" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4383,13 +4384,13 @@
         <v>167</v>
       </c>
       <c r="D103" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H103" t="s">
         <v>244</v>
       </c>
       <c r="I103" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4403,13 +4404,13 @@
         <v>169</v>
       </c>
       <c r="D104" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H104" t="s">
         <v>244</v>
       </c>
       <c r="I104" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4423,13 +4424,13 @@
         <v>171</v>
       </c>
       <c r="D105" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H105" t="s">
         <v>244</v>
       </c>
       <c r="I105" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4443,13 +4444,13 @@
         <v>173</v>
       </c>
       <c r="D106" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H106" t="s">
         <v>244</v>
       </c>
       <c r="I106" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4463,13 +4464,13 @@
         <v>175</v>
       </c>
       <c r="D107" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H107" t="s">
         <v>244</v>
       </c>
       <c r="I107" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4483,13 +4484,13 @@
         <v>177</v>
       </c>
       <c r="D108" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H108" t="s">
         <v>244</v>
       </c>
       <c r="I108" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4503,13 +4504,13 @@
         <v>179</v>
       </c>
       <c r="D109" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H109" t="s">
         <v>244</v>
       </c>
       <c r="I109" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4523,13 +4524,13 @@
         <v>181</v>
       </c>
       <c r="D110" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H110" t="s">
         <v>244</v>
       </c>
       <c r="I110" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4543,13 +4544,13 @@
         <v>183</v>
       </c>
       <c r="D111" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H111" t="s">
         <v>244</v>
       </c>
       <c r="I111" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4563,13 +4564,13 @@
         <v>185</v>
       </c>
       <c r="D112" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H112" t="s">
         <v>244</v>
       </c>
       <c r="I112" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4583,13 +4584,13 @@
         <v>188</v>
       </c>
       <c r="D113" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H113" t="s">
         <v>244</v>
       </c>
       <c r="I113" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4603,13 +4604,13 @@
         <v>190</v>
       </c>
       <c r="D114" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H114" t="s">
         <v>244</v>
       </c>
       <c r="I114" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4623,13 +4624,13 @@
         <v>192</v>
       </c>
       <c r="D115" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H115" t="s">
         <v>244</v>
       </c>
       <c r="I115" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4643,13 +4644,13 @@
         <v>194</v>
       </c>
       <c r="D116" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H116" t="s">
         <v>244</v>
       </c>
       <c r="I116" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4663,13 +4664,13 @@
         <v>196</v>
       </c>
       <c r="D117" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H117" t="s">
         <v>244</v>
       </c>
       <c r="I117" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4683,13 +4684,13 @@
         <v>198</v>
       </c>
       <c r="D118" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H118" t="s">
         <v>244</v>
       </c>
       <c r="I118" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4703,13 +4704,13 @@
         <v>200</v>
       </c>
       <c r="D119" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H119" t="s">
         <v>244</v>
       </c>
       <c r="I119" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4723,13 +4724,13 @@
         <v>201</v>
       </c>
       <c r="D120" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H120" t="s">
         <v>244</v>
       </c>
       <c r="I120" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4743,13 +4744,13 @@
         <v>202</v>
       </c>
       <c r="D121" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H121" t="s">
         <v>244</v>
       </c>
       <c r="I121" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4763,13 +4764,13 @@
         <v>203</v>
       </c>
       <c r="D122" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H122" t="s">
         <v>244</v>
       </c>
       <c r="I122" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4783,13 +4784,13 @@
         <v>204</v>
       </c>
       <c r="D123" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H123" t="s">
         <v>244</v>
       </c>
       <c r="I123" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4803,13 +4804,13 @@
         <v>205</v>
       </c>
       <c r="D124" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H124" t="s">
         <v>244</v>
       </c>
       <c r="I124" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4823,13 +4824,13 @@
         <v>207</v>
       </c>
       <c r="D125" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H125" t="s">
         <v>244</v>
       </c>
       <c r="I125" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4843,13 +4844,13 @@
         <v>208</v>
       </c>
       <c r="D126" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H126" t="s">
         <v>244</v>
       </c>
       <c r="I126" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4863,13 +4864,13 @@
         <v>209</v>
       </c>
       <c r="D127" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H127" t="s">
         <v>244</v>
       </c>
       <c r="I127" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4883,13 +4884,13 @@
         <v>210</v>
       </c>
       <c r="D128" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H128" t="s">
         <v>244</v>
       </c>
       <c r="I128" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4903,13 +4904,13 @@
         <v>211</v>
       </c>
       <c r="D129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H129" t="s">
         <v>244</v>
       </c>
       <c r="I129" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4923,13 +4924,13 @@
         <v>212</v>
       </c>
       <c r="D130" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H130" t="s">
         <v>244</v>
       </c>
       <c r="I130" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -4943,13 +4944,13 @@
         <v>214</v>
       </c>
       <c r="D131" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H131" t="s">
         <v>244</v>
       </c>
       <c r="I131" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -4963,13 +4964,13 @@
         <v>216</v>
       </c>
       <c r="D132" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H132" t="s">
         <v>244</v>
       </c>
       <c r="I132" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4983,13 +4984,13 @@
         <v>219</v>
       </c>
       <c r="D133" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H133" t="s">
         <v>244</v>
       </c>
       <c r="I133" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5003,13 +5004,13 @@
         <v>221</v>
       </c>
       <c r="D134" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H134" t="s">
         <v>244</v>
       </c>
       <c r="I134" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5023,13 +5024,13 @@
         <v>223</v>
       </c>
       <c r="D135" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H135" t="s">
         <v>244</v>
       </c>
       <c r="I135" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -5043,13 +5044,13 @@
         <v>225</v>
       </c>
       <c r="D136" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H136" t="s">
         <v>244</v>
       </c>
       <c r="I136" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5063,13 +5064,13 @@
         <v>227</v>
       </c>
       <c r="D137" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H137" t="s">
         <v>244</v>
       </c>
       <c r="I137" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5083,13 +5084,13 @@
         <v>230</v>
       </c>
       <c r="D138" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H138" t="s">
         <v>244</v>
       </c>
       <c r="I138" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -5103,13 +5104,13 @@
         <v>232</v>
       </c>
       <c r="D139" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H139" t="s">
         <v>244</v>
       </c>
       <c r="I139" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5123,13 +5124,13 @@
         <v>234</v>
       </c>
       <c r="D140" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H140" t="s">
         <v>244</v>
       </c>
       <c r="I140" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5143,13 +5144,13 @@
         <v>236</v>
       </c>
       <c r="D141" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H141" t="s">
         <v>244</v>
       </c>
       <c r="I141" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5157,19 +5158,19 @@
         <v>228</v>
       </c>
       <c r="B142" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C142" t="s">
         <v>237</v>
       </c>
       <c r="D142" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H142" t="s">
         <v>244</v>
       </c>
       <c r="I142" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5177,10 +5178,10 @@
         <v>228</v>
       </c>
       <c r="B143" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C143" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D143" t="s">
         <v>385</v>
@@ -5189,13 +5190,13 @@
         <v>3</v>
       </c>
       <c r="G143" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H143" t="s">
         <v>244</v>
       </c>
       <c r="I143" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5209,13 +5210,13 @@
         <v>239</v>
       </c>
       <c r="D144" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H144" t="s">
         <v>244</v>
       </c>
       <c r="I144" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -5229,13 +5230,13 @@
         <v>241</v>
       </c>
       <c r="D145" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H145" t="s">
         <v>244</v>
       </c>
       <c r="I145" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5249,13 +5250,13 @@
         <v>243</v>
       </c>
       <c r="D146" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H146" t="s">
         <v>244</v>
       </c>
       <c r="I146" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5275,7 +5276,7 @@
         <v>356</v>
       </c>
       <c r="I147" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5301,7 +5302,7 @@
         <v>356</v>
       </c>
       <c r="I148" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5321,7 +5322,7 @@
         <v>356</v>
       </c>
       <c r="I149" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5341,7 +5342,7 @@
         <v>356</v>
       </c>
       <c r="I150" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5361,7 +5362,7 @@
         <v>356</v>
       </c>
       <c r="I151" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5381,7 +5382,7 @@
         <v>356</v>
       </c>
       <c r="I152" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5407,7 +5408,7 @@
         <v>356</v>
       </c>
       <c r="I153" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5427,7 +5428,7 @@
         <v>356</v>
       </c>
       <c r="I154" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -5447,7 +5448,7 @@
         <v>356</v>
       </c>
       <c r="I155" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5473,7 +5474,7 @@
         <v>356</v>
       </c>
       <c r="I156" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5499,7 +5500,7 @@
         <v>356</v>
       </c>
       <c r="I157" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5519,7 +5520,7 @@
         <v>356</v>
       </c>
       <c r="I158" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5539,13 +5540,13 @@
         <v>5</v>
       </c>
       <c r="G159" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H159" t="s">
         <v>356</v>
       </c>
       <c r="I159" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5565,7 +5566,7 @@
         <v>356</v>
       </c>
       <c r="I160" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5585,7 +5586,7 @@
         <v>356</v>
       </c>
       <c r="I161" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5605,7 +5606,7 @@
         <v>356</v>
       </c>
       <c r="I162" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5631,7 +5632,7 @@
         <v>356</v>
       </c>
       <c r="I163" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -5654,13 +5655,13 @@
         <v>388</v>
       </c>
       <c r="G164" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H164" t="s">
         <v>356</v>
       </c>
       <c r="I164" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -5680,13 +5681,13 @@
         <v>5</v>
       </c>
       <c r="G165" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H165" t="s">
         <v>356</v>
       </c>
       <c r="I165" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5712,7 +5713,7 @@
         <v>356</v>
       </c>
       <c r="I166" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5723,7 +5724,7 @@
         <v>114</v>
       </c>
       <c r="C167" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D167" t="s">
         <v>385</v>
@@ -5732,13 +5733,13 @@
         <v>4</v>
       </c>
       <c r="G167" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H167" t="s">
         <v>356</v>
       </c>
       <c r="I167" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5764,7 +5765,7 @@
         <v>356</v>
       </c>
       <c r="I168" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5784,7 +5785,7 @@
         <v>356</v>
       </c>
       <c r="I169" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5804,7 +5805,7 @@
         <v>356</v>
       </c>
       <c r="I170" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5827,13 +5828,13 @@
         <v>388</v>
       </c>
       <c r="G171" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H171" t="s">
         <v>356</v>
       </c>
       <c r="I171" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5853,7 +5854,7 @@
         <v>356</v>
       </c>
       <c r="I172" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -5873,7 +5874,7 @@
         <v>356</v>
       </c>
       <c r="I173" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -5896,13 +5897,13 @@
         <v>388</v>
       </c>
       <c r="G174" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H174" t="s">
         <v>356</v>
       </c>
       <c r="I174" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -5922,7 +5923,7 @@
         <v>356</v>
       </c>
       <c r="I175" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -5942,7 +5943,7 @@
         <v>356</v>
       </c>
       <c r="I176" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -5956,13 +5957,13 @@
         <v>249</v>
       </c>
       <c r="D177" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H177" t="s">
         <v>356</v>
       </c>
       <c r="I177" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -5976,13 +5977,13 @@
         <v>251</v>
       </c>
       <c r="D178" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H178" t="s">
         <v>356</v>
       </c>
       <c r="I178" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -5996,13 +5997,13 @@
         <v>253</v>
       </c>
       <c r="D179" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H179" t="s">
         <v>356</v>
       </c>
       <c r="I179" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -6016,13 +6017,13 @@
         <v>255</v>
       </c>
       <c r="D180" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H180" t="s">
         <v>356</v>
       </c>
       <c r="I180" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -6036,13 +6037,13 @@
         <v>257</v>
       </c>
       <c r="D181" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H181" t="s">
         <v>356</v>
       </c>
       <c r="I181" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6056,13 +6057,13 @@
         <v>138</v>
       </c>
       <c r="D182" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H182" t="s">
         <v>356</v>
       </c>
       <c r="I182" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6076,13 +6077,13 @@
         <v>258</v>
       </c>
       <c r="D183" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H183" t="s">
         <v>356</v>
       </c>
       <c r="I183" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6096,13 +6097,13 @@
         <v>259</v>
       </c>
       <c r="D184" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H184" t="s">
         <v>356</v>
       </c>
       <c r="I184" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -6116,13 +6117,13 @@
         <v>407</v>
       </c>
       <c r="D185" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H185" t="s">
         <v>356</v>
       </c>
       <c r="I185" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6136,13 +6137,13 @@
         <v>147</v>
       </c>
       <c r="D186" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H186" t="s">
         <v>356</v>
       </c>
       <c r="I186" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6156,13 +6157,13 @@
         <v>149</v>
       </c>
       <c r="D187" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H187" t="s">
         <v>356</v>
       </c>
       <c r="I187" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6176,13 +6177,13 @@
         <v>260</v>
       </c>
       <c r="D188" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H188" t="s">
         <v>356</v>
       </c>
       <c r="I188" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6196,13 +6197,13 @@
         <v>261</v>
       </c>
       <c r="D189" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H189" t="s">
         <v>356</v>
       </c>
       <c r="I189" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6216,13 +6217,13 @@
         <v>262</v>
       </c>
       <c r="D190" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H190" t="s">
         <v>356</v>
       </c>
       <c r="I190" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -6236,13 +6237,13 @@
         <v>157</v>
       </c>
       <c r="D191" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H191" t="s">
         <v>356</v>
       </c>
       <c r="I191" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -6256,13 +6257,13 @@
         <v>408</v>
       </c>
       <c r="D192" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H192" t="s">
         <v>356</v>
       </c>
       <c r="I192" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6276,13 +6277,13 @@
         <v>160</v>
       </c>
       <c r="D193" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H193" t="s">
         <v>356</v>
       </c>
       <c r="I193" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6296,13 +6297,13 @@
         <v>162</v>
       </c>
       <c r="D194" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H194" t="s">
         <v>356</v>
       </c>
       <c r="I194" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6316,13 +6317,13 @@
         <v>266</v>
       </c>
       <c r="D195" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H195" t="s">
         <v>356</v>
       </c>
       <c r="I195" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6336,13 +6337,13 @@
         <v>179</v>
       </c>
       <c r="D196" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H196" t="s">
         <v>356</v>
       </c>
       <c r="I196" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -6356,13 +6357,13 @@
         <v>181</v>
       </c>
       <c r="D197" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H197" t="s">
         <v>356</v>
       </c>
       <c r="I197" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6376,13 +6377,13 @@
         <v>183</v>
       </c>
       <c r="D198" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H198" t="s">
         <v>356</v>
       </c>
       <c r="I198" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6396,13 +6397,13 @@
         <v>185</v>
       </c>
       <c r="D199" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H199" t="s">
         <v>356</v>
       </c>
       <c r="I199" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -6416,13 +6417,13 @@
         <v>269</v>
       </c>
       <c r="D200" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H200" t="s">
         <v>356</v>
       </c>
       <c r="I200" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6436,13 +6437,13 @@
         <v>272</v>
       </c>
       <c r="D201" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H201" t="s">
         <v>356</v>
       </c>
       <c r="I201" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6456,13 +6457,13 @@
         <v>274</v>
       </c>
       <c r="D202" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H202" t="s">
         <v>356</v>
       </c>
       <c r="I202" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6476,13 +6477,13 @@
         <v>276</v>
       </c>
       <c r="D203" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H203" t="s">
         <v>356</v>
       </c>
       <c r="I203" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -6496,13 +6497,13 @@
         <v>278</v>
       </c>
       <c r="D204" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H204" t="s">
         <v>356</v>
       </c>
       <c r="I204" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6516,13 +6517,13 @@
         <v>280</v>
       </c>
       <c r="D205" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H205" t="s">
         <v>356</v>
       </c>
       <c r="I205" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -6536,13 +6537,13 @@
         <v>282</v>
       </c>
       <c r="D206" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H206" t="s">
         <v>356</v>
       </c>
       <c r="I206" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -6556,13 +6557,13 @@
         <v>284</v>
       </c>
       <c r="D207" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H207" t="s">
         <v>356</v>
       </c>
       <c r="I207" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6576,13 +6577,13 @@
         <v>286</v>
       </c>
       <c r="D208" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H208" t="s">
         <v>356</v>
       </c>
       <c r="I208" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -6596,13 +6597,13 @@
         <v>288</v>
       </c>
       <c r="D209" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H209" t="s">
         <v>356</v>
       </c>
       <c r="I209" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -6616,13 +6617,13 @@
         <v>290</v>
       </c>
       <c r="D210" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H210" t="s">
         <v>356</v>
       </c>
       <c r="I210" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -6636,13 +6637,13 @@
         <v>292</v>
       </c>
       <c r="D211" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H211" t="s">
         <v>356</v>
       </c>
       <c r="I211" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -6656,13 +6657,13 @@
         <v>188</v>
       </c>
       <c r="D212" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H212" t="s">
         <v>356</v>
       </c>
       <c r="I212" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -6676,13 +6677,13 @@
         <v>190</v>
       </c>
       <c r="D213" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H213" t="s">
         <v>356</v>
       </c>
       <c r="I213" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -6696,13 +6697,13 @@
         <v>192</v>
       </c>
       <c r="D214" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H214" t="s">
         <v>356</v>
       </c>
       <c r="I214" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -6716,13 +6717,13 @@
         <v>194</v>
       </c>
       <c r="D215" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H215" t="s">
         <v>356</v>
       </c>
       <c r="I215" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -6736,13 +6737,13 @@
         <v>196</v>
       </c>
       <c r="D216" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H216" t="s">
         <v>356</v>
       </c>
       <c r="I216" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -6756,13 +6757,13 @@
         <v>198</v>
       </c>
       <c r="D217" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H217" t="s">
         <v>356</v>
       </c>
       <c r="I217" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -6776,13 +6777,13 @@
         <v>200</v>
       </c>
       <c r="D218" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H218" t="s">
         <v>356</v>
       </c>
       <c r="I218" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
@@ -6796,13 +6797,13 @@
         <v>201</v>
       </c>
       <c r="D219" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H219" t="s">
         <v>356</v>
       </c>
       <c r="I219" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -6816,13 +6817,13 @@
         <v>202</v>
       </c>
       <c r="D220" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H220" t="s">
         <v>356</v>
       </c>
       <c r="I220" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -6836,13 +6837,13 @@
         <v>203</v>
       </c>
       <c r="D221" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H221" t="s">
         <v>356</v>
       </c>
       <c r="I221" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -6856,13 +6857,13 @@
         <v>204</v>
       </c>
       <c r="D222" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H222" t="s">
         <v>356</v>
       </c>
       <c r="I222" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -6876,13 +6877,13 @@
         <v>205</v>
       </c>
       <c r="D223" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H223" t="s">
         <v>356</v>
       </c>
       <c r="I223" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -6896,13 +6897,13 @@
         <v>207</v>
       </c>
       <c r="D224" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H224" t="s">
         <v>356</v>
       </c>
       <c r="I224" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -6916,13 +6917,13 @@
         <v>208</v>
       </c>
       <c r="D225" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H225" t="s">
         <v>356</v>
       </c>
       <c r="I225" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -6936,13 +6937,13 @@
         <v>209</v>
       </c>
       <c r="D226" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H226" t="s">
         <v>356</v>
       </c>
       <c r="I226" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -6956,13 +6957,13 @@
         <v>210</v>
       </c>
       <c r="D227" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H227" t="s">
         <v>356</v>
       </c>
       <c r="I227" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -6976,13 +6977,13 @@
         <v>211</v>
       </c>
       <c r="D228" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H228" t="s">
         <v>356</v>
       </c>
       <c r="I228" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -6996,13 +6997,13 @@
         <v>212</v>
       </c>
       <c r="D229" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H229" t="s">
         <v>356</v>
       </c>
       <c r="I229" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7022,7 +7023,7 @@
         <v>356</v>
       </c>
       <c r="I230" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -7042,7 +7043,7 @@
         <v>356</v>
       </c>
       <c r="I231" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -7062,7 +7063,7 @@
         <v>356</v>
       </c>
       <c r="I232" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7082,7 +7083,7 @@
         <v>356</v>
       </c>
       <c r="I233" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
@@ -7102,7 +7103,7 @@
         <v>356</v>
       </c>
       <c r="I234" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -7122,7 +7123,7 @@
         <v>356</v>
       </c>
       <c r="I235" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -7142,7 +7143,7 @@
         <v>356</v>
       </c>
       <c r="I236" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -7162,7 +7163,7 @@
         <v>356</v>
       </c>
       <c r="I237" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -7182,7 +7183,7 @@
         <v>356</v>
       </c>
       <c r="I238" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -7202,7 +7203,7 @@
         <v>356</v>
       </c>
       <c r="I239" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
@@ -7222,7 +7223,7 @@
         <v>356</v>
       </c>
       <c r="I240" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
@@ -7242,7 +7243,7 @@
         <v>356</v>
       </c>
       <c r="I241" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -7262,7 +7263,7 @@
         <v>356</v>
       </c>
       <c r="I242" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
@@ -7282,7 +7283,7 @@
         <v>356</v>
       </c>
       <c r="I243" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
@@ -7302,7 +7303,7 @@
         <v>356</v>
       </c>
       <c r="I244" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
@@ -7322,7 +7323,7 @@
         <v>356</v>
       </c>
       <c r="I245" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
@@ -7342,7 +7343,7 @@
         <v>356</v>
       </c>
       <c r="I246" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
@@ -7362,7 +7363,7 @@
         <v>356</v>
       </c>
       <c r="I247" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
@@ -7382,7 +7383,7 @@
         <v>356</v>
       </c>
       <c r="I248" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
@@ -7402,7 +7403,7 @@
         <v>356</v>
       </c>
       <c r="I249" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
@@ -7422,7 +7423,7 @@
         <v>356</v>
       </c>
       <c r="I250" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
@@ -7442,7 +7443,7 @@
         <v>356</v>
       </c>
       <c r="I251" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
@@ -7462,7 +7463,7 @@
         <v>356</v>
       </c>
       <c r="I252" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
@@ -7482,7 +7483,7 @@
         <v>356</v>
       </c>
       <c r="I253" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
@@ -7502,7 +7503,7 @@
         <v>356</v>
       </c>
       <c r="I254" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
@@ -7522,7 +7523,7 @@
         <v>356</v>
       </c>
       <c r="I255" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
@@ -7542,7 +7543,7 @@
         <v>356</v>
       </c>
       <c r="I256" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
@@ -7562,7 +7563,7 @@
         <v>356</v>
       </c>
       <c r="I257" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
@@ -7582,7 +7583,7 @@
         <v>356</v>
       </c>
       <c r="I258" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
@@ -7602,7 +7603,7 @@
         <v>356</v>
       </c>
       <c r="I259" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
@@ -7622,7 +7623,7 @@
         <v>356</v>
       </c>
       <c r="I260" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
@@ -7642,7 +7643,7 @@
         <v>81</v>
       </c>
       <c r="I261" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
@@ -7662,7 +7663,7 @@
         <v>81</v>
       </c>
       <c r="I262" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
@@ -7682,7 +7683,7 @@
         <v>81</v>
       </c>
       <c r="I263" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
@@ -7702,7 +7703,7 @@
         <v>81</v>
       </c>
       <c r="I264" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
@@ -7722,7 +7723,7 @@
         <v>81</v>
       </c>
       <c r="I265" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
@@ -7742,7 +7743,7 @@
         <v>81</v>
       </c>
       <c r="I266" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
@@ -7762,7 +7763,7 @@
         <v>81</v>
       </c>
       <c r="I267" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
@@ -7782,7 +7783,7 @@
         <v>81</v>
       </c>
       <c r="I268" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
@@ -7802,7 +7803,7 @@
         <v>81</v>
       </c>
       <c r="I269" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
@@ -7822,7 +7823,7 @@
         <v>81</v>
       </c>
       <c r="I270" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
@@ -7833,7 +7834,7 @@
         <v>431</v>
       </c>
       <c r="C271" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D271" t="s">
         <v>375</v>
@@ -7842,7 +7843,7 @@
         <v>81</v>
       </c>
       <c r="I271" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
@@ -7862,7 +7863,7 @@
         <v>81</v>
       </c>
       <c r="I272" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
@@ -7882,7 +7883,7 @@
         <v>81</v>
       </c>
       <c r="I273" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
@@ -7902,7 +7903,7 @@
         <v>81</v>
       </c>
       <c r="I274" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
@@ -7922,7 +7923,7 @@
         <v>81</v>
       </c>
       <c r="I275" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
@@ -7942,7 +7943,7 @@
         <v>81</v>
       </c>
       <c r="I276" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
@@ -7962,7 +7963,7 @@
         <v>81</v>
       </c>
       <c r="I277" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
@@ -7982,7 +7983,7 @@
         <v>81</v>
       </c>
       <c r="I278" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
@@ -7990,7 +7991,7 @@
         <v>362</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>39</v>
@@ -8002,7 +8003,7 @@
         <v>81</v>
       </c>
       <c r="I279" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated 'add definition' listbox
</commit_message>
<xml_diff>
--- a/data/method_fragments/master_list.xlsx
+++ b/data/method_fragments/master_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiny\ IA-Tool-V1\data\method_fragments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD8EF1F-A060-4ABC-BC05-DD40A20BDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AE508E-0431-4A9E-9BEE-1C9DC20C7E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{617BE651-D097-4A39-BC0E-E2962D9C7834}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="487">
   <si>
     <t>category</t>
   </si>
@@ -1863,6 +1863,12 @@
   </si>
   <si>
     <t>User satisfaction smartphone 4</t>
+  </si>
+  <si>
+    <t>strongly disagree;  disagree;  somewhat disagree;  neither agree or disagree;  somewhat agree;  agree;  strongly agree</t>
+  </si>
+  <si>
+    <t>I need a lot of additional knowledge about the topic;  I need some additional knowledge about the topic ;  I need a little additional knowledge about the topic ;  I have some knowledge about the topic ;  I have good knowledge about the topic ;  I have strong knowledge about the topic</t>
   </si>
 </sst>
 </file>
@@ -2244,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF63B7-F4D5-4739-85BC-BBDBC70D9D30}">
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4042,6 +4048,9 @@
       <c r="D84" t="s">
         <v>465</v>
       </c>
+      <c r="G84" t="s">
+        <v>485</v>
+      </c>
       <c r="H84" t="s">
         <v>238</v>
       </c>
@@ -4062,6 +4071,9 @@
       <c r="D85" t="s">
         <v>465</v>
       </c>
+      <c r="G85" t="s">
+        <v>485</v>
+      </c>
       <c r="H85" t="s">
         <v>238</v>
       </c>
@@ -4082,6 +4094,9 @@
       <c r="D86" t="s">
         <v>465</v>
       </c>
+      <c r="G86" t="s">
+        <v>485</v>
+      </c>
       <c r="H86" t="s">
         <v>238</v>
       </c>
@@ -4102,6 +4117,9 @@
       <c r="D87" t="s">
         <v>465</v>
       </c>
+      <c r="G87" t="s">
+        <v>485</v>
+      </c>
       <c r="H87" t="s">
         <v>238</v>
       </c>
@@ -4122,6 +4140,9 @@
       <c r="D88" t="s">
         <v>465</v>
       </c>
+      <c r="G88" t="s">
+        <v>485</v>
+      </c>
       <c r="H88" t="s">
         <v>238</v>
       </c>
@@ -4142,6 +4163,9 @@
       <c r="D89" t="s">
         <v>465</v>
       </c>
+      <c r="G89" t="s">
+        <v>485</v>
+      </c>
       <c r="H89" t="s">
         <v>238</v>
       </c>
@@ -4162,6 +4186,9 @@
       <c r="D90" t="s">
         <v>465</v>
       </c>
+      <c r="G90" t="s">
+        <v>485</v>
+      </c>
       <c r="H90" t="s">
         <v>238</v>
       </c>
@@ -4182,6 +4209,9 @@
       <c r="D91" t="s">
         <v>465</v>
       </c>
+      <c r="G91" t="s">
+        <v>485</v>
+      </c>
       <c r="H91" t="s">
         <v>238</v>
       </c>
@@ -4202,6 +4232,9 @@
       <c r="D92" t="s">
         <v>465</v>
       </c>
+      <c r="G92" t="s">
+        <v>485</v>
+      </c>
       <c r="H92" t="s">
         <v>238</v>
       </c>
@@ -4222,6 +4255,9 @@
       <c r="D93" t="s">
         <v>465</v>
       </c>
+      <c r="G93" t="s">
+        <v>485</v>
+      </c>
       <c r="H93" t="s">
         <v>238</v>
       </c>
@@ -4242,6 +4278,9 @@
       <c r="D94" t="s">
         <v>465</v>
       </c>
+      <c r="G94" t="s">
+        <v>485</v>
+      </c>
       <c r="H94" t="s">
         <v>238</v>
       </c>
@@ -4262,6 +4301,9 @@
       <c r="D95" t="s">
         <v>465</v>
       </c>
+      <c r="G95" t="s">
+        <v>485</v>
+      </c>
       <c r="H95" t="s">
         <v>238</v>
       </c>
@@ -4282,6 +4324,9 @@
       <c r="D96" t="s">
         <v>465</v>
       </c>
+      <c r="G96" t="s">
+        <v>485</v>
+      </c>
       <c r="H96" t="s">
         <v>238</v>
       </c>
@@ -4302,6 +4347,9 @@
       <c r="D97" t="s">
         <v>465</v>
       </c>
+      <c r="G97" t="s">
+        <v>485</v>
+      </c>
       <c r="H97" t="s">
         <v>238</v>
       </c>
@@ -4322,6 +4370,9 @@
       <c r="D98" t="s">
         <v>465</v>
       </c>
+      <c r="G98" t="s">
+        <v>485</v>
+      </c>
       <c r="H98" t="s">
         <v>238</v>
       </c>
@@ -4342,6 +4393,9 @@
       <c r="D99" t="s">
         <v>465</v>
       </c>
+      <c r="G99" t="s">
+        <v>485</v>
+      </c>
       <c r="H99" t="s">
         <v>238</v>
       </c>
@@ -4362,6 +4416,9 @@
       <c r="D100" t="s">
         <v>465</v>
       </c>
+      <c r="G100" t="s">
+        <v>485</v>
+      </c>
       <c r="H100" t="s">
         <v>238</v>
       </c>
@@ -4382,6 +4439,9 @@
       <c r="D101" t="s">
         <v>465</v>
       </c>
+      <c r="G101" t="s">
+        <v>485</v>
+      </c>
       <c r="H101" t="s">
         <v>238</v>
       </c>
@@ -4402,6 +4462,9 @@
       <c r="D102" t="s">
         <v>465</v>
       </c>
+      <c r="G102" t="s">
+        <v>485</v>
+      </c>
       <c r="H102" t="s">
         <v>238</v>
       </c>
@@ -4422,6 +4485,9 @@
       <c r="D103" t="s">
         <v>465</v>
       </c>
+      <c r="G103" t="s">
+        <v>485</v>
+      </c>
       <c r="H103" t="s">
         <v>238</v>
       </c>
@@ -4442,6 +4508,9 @@
       <c r="D104" t="s">
         <v>465</v>
       </c>
+      <c r="G104" t="s">
+        <v>485</v>
+      </c>
       <c r="H104" t="s">
         <v>238</v>
       </c>
@@ -4462,6 +4531,9 @@
       <c r="D105" t="s">
         <v>465</v>
       </c>
+      <c r="G105" t="s">
+        <v>485</v>
+      </c>
       <c r="H105" t="s">
         <v>238</v>
       </c>
@@ -4482,6 +4554,9 @@
       <c r="D106" t="s">
         <v>465</v>
       </c>
+      <c r="G106" t="s">
+        <v>485</v>
+      </c>
       <c r="H106" t="s">
         <v>238</v>
       </c>
@@ -4502,6 +4577,9 @@
       <c r="D107" t="s">
         <v>465</v>
       </c>
+      <c r="G107" t="s">
+        <v>485</v>
+      </c>
       <c r="H107" t="s">
         <v>238</v>
       </c>
@@ -4522,6 +4600,9 @@
       <c r="D108" t="s">
         <v>465</v>
       </c>
+      <c r="G108" t="s">
+        <v>485</v>
+      </c>
       <c r="H108" t="s">
         <v>238</v>
       </c>
@@ -4542,6 +4623,9 @@
       <c r="D109" t="s">
         <v>465</v>
       </c>
+      <c r="G109" t="s">
+        <v>485</v>
+      </c>
       <c r="H109" t="s">
         <v>238</v>
       </c>
@@ -4562,6 +4646,9 @@
       <c r="D110" t="s">
         <v>465</v>
       </c>
+      <c r="G110" t="s">
+        <v>485</v>
+      </c>
       <c r="H110" t="s">
         <v>238</v>
       </c>
@@ -4582,6 +4669,9 @@
       <c r="D111" t="s">
         <v>465</v>
       </c>
+      <c r="G111" t="s">
+        <v>485</v>
+      </c>
       <c r="H111" t="s">
         <v>238</v>
       </c>
@@ -4602,6 +4692,9 @@
       <c r="D112" t="s">
         <v>465</v>
       </c>
+      <c r="G112" t="s">
+        <v>485</v>
+      </c>
       <c r="H112" t="s">
         <v>238</v>
       </c>
@@ -4622,6 +4715,9 @@
       <c r="D113" t="s">
         <v>465</v>
       </c>
+      <c r="G113" t="s">
+        <v>485</v>
+      </c>
       <c r="H113" t="s">
         <v>238</v>
       </c>
@@ -4642,6 +4738,9 @@
       <c r="D114" t="s">
         <v>465</v>
       </c>
+      <c r="G114" t="s">
+        <v>485</v>
+      </c>
       <c r="H114" t="s">
         <v>238</v>
       </c>
@@ -4662,6 +4761,9 @@
       <c r="D115" t="s">
         <v>465</v>
       </c>
+      <c r="G115" t="s">
+        <v>485</v>
+      </c>
       <c r="H115" t="s">
         <v>238</v>
       </c>
@@ -4682,6 +4784,9 @@
       <c r="D116" t="s">
         <v>465</v>
       </c>
+      <c r="G116" t="s">
+        <v>485</v>
+      </c>
       <c r="H116" t="s">
         <v>238</v>
       </c>
@@ -4702,6 +4807,9 @@
       <c r="D117" t="s">
         <v>465</v>
       </c>
+      <c r="G117" t="s">
+        <v>485</v>
+      </c>
       <c r="H117" t="s">
         <v>238</v>
       </c>
@@ -4722,6 +4830,9 @@
       <c r="D118" t="s">
         <v>465</v>
       </c>
+      <c r="G118" t="s">
+        <v>485</v>
+      </c>
       <c r="H118" t="s">
         <v>238</v>
       </c>
@@ -4742,6 +4853,9 @@
       <c r="D119" t="s">
         <v>465</v>
       </c>
+      <c r="G119" t="s">
+        <v>485</v>
+      </c>
       <c r="H119" t="s">
         <v>238</v>
       </c>
@@ -4762,6 +4876,9 @@
       <c r="D120" t="s">
         <v>465</v>
       </c>
+      <c r="G120" t="s">
+        <v>485</v>
+      </c>
       <c r="H120" t="s">
         <v>238</v>
       </c>
@@ -4782,6 +4899,9 @@
       <c r="D121" t="s">
         <v>465</v>
       </c>
+      <c r="G121" t="s">
+        <v>485</v>
+      </c>
       <c r="H121" t="s">
         <v>238</v>
       </c>
@@ -4802,6 +4922,9 @@
       <c r="D122" t="s">
         <v>465</v>
       </c>
+      <c r="G122" t="s">
+        <v>485</v>
+      </c>
       <c r="H122" t="s">
         <v>238</v>
       </c>
@@ -4822,6 +4945,9 @@
       <c r="D123" t="s">
         <v>465</v>
       </c>
+      <c r="G123" t="s">
+        <v>485</v>
+      </c>
       <c r="H123" t="s">
         <v>238</v>
       </c>
@@ -4842,6 +4968,9 @@
       <c r="D124" t="s">
         <v>465</v>
       </c>
+      <c r="G124" t="s">
+        <v>485</v>
+      </c>
       <c r="H124" t="s">
         <v>238</v>
       </c>
@@ -4862,6 +4991,9 @@
       <c r="D125" t="s">
         <v>465</v>
       </c>
+      <c r="G125" t="s">
+        <v>485</v>
+      </c>
       <c r="H125" t="s">
         <v>238</v>
       </c>
@@ -4882,6 +5014,9 @@
       <c r="D126" t="s">
         <v>465</v>
       </c>
+      <c r="G126" t="s">
+        <v>485</v>
+      </c>
       <c r="H126" t="s">
         <v>238</v>
       </c>
@@ -4902,6 +5037,9 @@
       <c r="D127" t="s">
         <v>465</v>
       </c>
+      <c r="G127" t="s">
+        <v>485</v>
+      </c>
       <c r="H127" t="s">
         <v>238</v>
       </c>
@@ -4922,6 +5060,9 @@
       <c r="D128" t="s">
         <v>465</v>
       </c>
+      <c r="G128" t="s">
+        <v>485</v>
+      </c>
       <c r="H128" t="s">
         <v>238</v>
       </c>
@@ -4942,6 +5083,9 @@
       <c r="D129" t="s">
         <v>465</v>
       </c>
+      <c r="G129" t="s">
+        <v>485</v>
+      </c>
       <c r="H129" t="s">
         <v>238</v>
       </c>
@@ -4962,6 +5106,9 @@
       <c r="D130" t="s">
         <v>465</v>
       </c>
+      <c r="G130" t="s">
+        <v>485</v>
+      </c>
       <c r="H130" t="s">
         <v>238</v>
       </c>
@@ -4982,6 +5129,9 @@
       <c r="D131" t="s">
         <v>465</v>
       </c>
+      <c r="G131" t="s">
+        <v>485</v>
+      </c>
       <c r="H131" t="s">
         <v>238</v>
       </c>
@@ -5002,6 +5152,9 @@
       <c r="D132" t="s">
         <v>465</v>
       </c>
+      <c r="G132" t="s">
+        <v>485</v>
+      </c>
       <c r="H132" t="s">
         <v>238</v>
       </c>
@@ -5022,6 +5175,9 @@
       <c r="D133" t="s">
         <v>465</v>
       </c>
+      <c r="G133" t="s">
+        <v>485</v>
+      </c>
       <c r="H133" t="s">
         <v>238</v>
       </c>
@@ -5042,6 +5198,9 @@
       <c r="D134" t="s">
         <v>465</v>
       </c>
+      <c r="G134" t="s">
+        <v>485</v>
+      </c>
       <c r="H134" t="s">
         <v>238</v>
       </c>
@@ -5062,6 +5221,9 @@
       <c r="D135" t="s">
         <v>465</v>
       </c>
+      <c r="G135" t="s">
+        <v>485</v>
+      </c>
       <c r="H135" t="s">
         <v>238</v>
       </c>
@@ -5082,6 +5244,9 @@
       <c r="D136" t="s">
         <v>465</v>
       </c>
+      <c r="G136" t="s">
+        <v>485</v>
+      </c>
       <c r="H136" t="s">
         <v>238</v>
       </c>
@@ -5102,6 +5267,9 @@
       <c r="D137" t="s">
         <v>465</v>
       </c>
+      <c r="G137" t="s">
+        <v>485</v>
+      </c>
       <c r="H137" t="s">
         <v>238</v>
       </c>
@@ -5122,6 +5290,9 @@
       <c r="D138" t="s">
         <v>465</v>
       </c>
+      <c r="G138" t="s">
+        <v>485</v>
+      </c>
       <c r="H138" t="s">
         <v>238</v>
       </c>
@@ -5142,6 +5313,9 @@
       <c r="D139" t="s">
         <v>465</v>
       </c>
+      <c r="G139" t="s">
+        <v>485</v>
+      </c>
       <c r="H139" t="s">
         <v>238</v>
       </c>
@@ -5162,6 +5336,9 @@
       <c r="D140" t="s">
         <v>465</v>
       </c>
+      <c r="G140" t="s">
+        <v>485</v>
+      </c>
       <c r="H140" t="s">
         <v>238</v>
       </c>
@@ -5182,6 +5359,9 @@
       <c r="D141" t="s">
         <v>465</v>
       </c>
+      <c r="G141" t="s">
+        <v>485</v>
+      </c>
       <c r="H141" t="s">
         <v>238</v>
       </c>
@@ -5202,6 +5382,9 @@
       <c r="D142" t="s">
         <v>465</v>
       </c>
+      <c r="G142" t="s">
+        <v>485</v>
+      </c>
       <c r="H142" t="s">
         <v>238</v>
       </c>
@@ -5248,6 +5431,9 @@
       <c r="D144" t="s">
         <v>465</v>
       </c>
+      <c r="G144" t="s">
+        <v>485</v>
+      </c>
       <c r="H144" t="s">
         <v>238</v>
       </c>
@@ -5268,6 +5454,9 @@
       <c r="D145" t="s">
         <v>465</v>
       </c>
+      <c r="G145" t="s">
+        <v>485</v>
+      </c>
       <c r="H145" t="s">
         <v>238</v>
       </c>
@@ -5288,6 +5477,9 @@
       <c r="D146" t="s">
         <v>465</v>
       </c>
+      <c r="G146" t="s">
+        <v>485</v>
+      </c>
       <c r="H146" t="s">
         <v>238</v>
       </c>
@@ -5995,6 +6187,9 @@
       <c r="D177" t="s">
         <v>465</v>
       </c>
+      <c r="G177" t="s">
+        <v>485</v>
+      </c>
       <c r="H177" t="s">
         <v>350</v>
       </c>
@@ -6015,6 +6210,9 @@
       <c r="D178" t="s">
         <v>465</v>
       </c>
+      <c r="G178" t="s">
+        <v>485</v>
+      </c>
       <c r="H178" t="s">
         <v>350</v>
       </c>
@@ -6035,6 +6233,9 @@
       <c r="D179" t="s">
         <v>465</v>
       </c>
+      <c r="G179" t="s">
+        <v>485</v>
+      </c>
       <c r="H179" t="s">
         <v>350</v>
       </c>
@@ -6055,6 +6256,9 @@
       <c r="D180" t="s">
         <v>465</v>
       </c>
+      <c r="G180" t="s">
+        <v>485</v>
+      </c>
       <c r="H180" t="s">
         <v>350</v>
       </c>
@@ -6075,6 +6279,9 @@
       <c r="D181" t="s">
         <v>465</v>
       </c>
+      <c r="G181" t="s">
+        <v>485</v>
+      </c>
       <c r="H181" t="s">
         <v>350</v>
       </c>
@@ -6095,6 +6302,9 @@
       <c r="D182" t="s">
         <v>465</v>
       </c>
+      <c r="G182" t="s">
+        <v>485</v>
+      </c>
       <c r="H182" t="s">
         <v>350</v>
       </c>
@@ -6115,6 +6325,9 @@
       <c r="D183" t="s">
         <v>465</v>
       </c>
+      <c r="G183" t="s">
+        <v>485</v>
+      </c>
       <c r="H183" t="s">
         <v>350</v>
       </c>
@@ -6135,6 +6348,9 @@
       <c r="D184" t="s">
         <v>465</v>
       </c>
+      <c r="G184" t="s">
+        <v>485</v>
+      </c>
       <c r="H184" t="s">
         <v>350</v>
       </c>
@@ -6155,6 +6371,9 @@
       <c r="D185" t="s">
         <v>465</v>
       </c>
+      <c r="G185" t="s">
+        <v>485</v>
+      </c>
       <c r="H185" t="s">
         <v>350</v>
       </c>
@@ -6175,6 +6394,9 @@
       <c r="D186" t="s">
         <v>465</v>
       </c>
+      <c r="G186" t="s">
+        <v>485</v>
+      </c>
       <c r="H186" t="s">
         <v>350</v>
       </c>
@@ -6195,6 +6417,9 @@
       <c r="D187" t="s">
         <v>465</v>
       </c>
+      <c r="G187" t="s">
+        <v>485</v>
+      </c>
       <c r="H187" t="s">
         <v>350</v>
       </c>
@@ -6215,6 +6440,9 @@
       <c r="D188" t="s">
         <v>465</v>
       </c>
+      <c r="G188" t="s">
+        <v>485</v>
+      </c>
       <c r="H188" t="s">
         <v>350</v>
       </c>
@@ -6235,6 +6463,9 @@
       <c r="D189" t="s">
         <v>465</v>
       </c>
+      <c r="G189" t="s">
+        <v>485</v>
+      </c>
       <c r="H189" t="s">
         <v>350</v>
       </c>
@@ -6255,6 +6486,9 @@
       <c r="D190" t="s">
         <v>465</v>
       </c>
+      <c r="G190" t="s">
+        <v>485</v>
+      </c>
       <c r="H190" t="s">
         <v>350</v>
       </c>
@@ -6275,6 +6509,9 @@
       <c r="D191" t="s">
         <v>465</v>
       </c>
+      <c r="G191" t="s">
+        <v>485</v>
+      </c>
       <c r="H191" t="s">
         <v>350</v>
       </c>
@@ -6295,6 +6532,9 @@
       <c r="D192" t="s">
         <v>465</v>
       </c>
+      <c r="G192" t="s">
+        <v>485</v>
+      </c>
       <c r="H192" t="s">
         <v>350</v>
       </c>
@@ -6315,6 +6555,9 @@
       <c r="D193" t="s">
         <v>465</v>
       </c>
+      <c r="G193" t="s">
+        <v>485</v>
+      </c>
       <c r="H193" t="s">
         <v>350</v>
       </c>
@@ -6335,6 +6578,9 @@
       <c r="D194" t="s">
         <v>465</v>
       </c>
+      <c r="G194" t="s">
+        <v>485</v>
+      </c>
       <c r="H194" t="s">
         <v>350</v>
       </c>
@@ -6355,6 +6601,9 @@
       <c r="D195" t="s">
         <v>465</v>
       </c>
+      <c r="G195" t="s">
+        <v>485</v>
+      </c>
       <c r="H195" t="s">
         <v>350</v>
       </c>
@@ -6375,6 +6624,9 @@
       <c r="D196" t="s">
         <v>465</v>
       </c>
+      <c r="G196" t="s">
+        <v>485</v>
+      </c>
       <c r="H196" t="s">
         <v>350</v>
       </c>
@@ -6395,6 +6647,9 @@
       <c r="D197" t="s">
         <v>465</v>
       </c>
+      <c r="G197" t="s">
+        <v>485</v>
+      </c>
       <c r="H197" t="s">
         <v>350</v>
       </c>
@@ -6415,6 +6670,9 @@
       <c r="D198" t="s">
         <v>465</v>
       </c>
+      <c r="G198" t="s">
+        <v>485</v>
+      </c>
       <c r="H198" t="s">
         <v>350</v>
       </c>
@@ -6435,6 +6693,9 @@
       <c r="D199" t="s">
         <v>465</v>
       </c>
+      <c r="G199" t="s">
+        <v>485</v>
+      </c>
       <c r="H199" t="s">
         <v>350</v>
       </c>
@@ -6455,6 +6716,9 @@
       <c r="D200" t="s">
         <v>465</v>
       </c>
+      <c r="G200" t="s">
+        <v>485</v>
+      </c>
       <c r="H200" t="s">
         <v>350</v>
       </c>
@@ -6475,6 +6739,9 @@
       <c r="D201" t="s">
         <v>465</v>
       </c>
+      <c r="G201" t="s">
+        <v>485</v>
+      </c>
       <c r="H201" t="s">
         <v>350</v>
       </c>
@@ -6495,6 +6762,9 @@
       <c r="D202" t="s">
         <v>465</v>
       </c>
+      <c r="G202" t="s">
+        <v>485</v>
+      </c>
       <c r="H202" t="s">
         <v>350</v>
       </c>
@@ -6515,6 +6785,9 @@
       <c r="D203" t="s">
         <v>465</v>
       </c>
+      <c r="G203" t="s">
+        <v>485</v>
+      </c>
       <c r="H203" t="s">
         <v>350</v>
       </c>
@@ -6535,6 +6808,9 @@
       <c r="D204" t="s">
         <v>465</v>
       </c>
+      <c r="G204" t="s">
+        <v>485</v>
+      </c>
       <c r="H204" t="s">
         <v>350</v>
       </c>
@@ -6555,6 +6831,9 @@
       <c r="D205" t="s">
         <v>465</v>
       </c>
+      <c r="G205" t="s">
+        <v>485</v>
+      </c>
       <c r="H205" t="s">
         <v>350</v>
       </c>
@@ -6575,6 +6854,9 @@
       <c r="D206" t="s">
         <v>465</v>
       </c>
+      <c r="G206" t="s">
+        <v>485</v>
+      </c>
       <c r="H206" t="s">
         <v>350</v>
       </c>
@@ -6595,6 +6877,9 @@
       <c r="D207" t="s">
         <v>465</v>
       </c>
+      <c r="G207" t="s">
+        <v>485</v>
+      </c>
       <c r="H207" t="s">
         <v>350</v>
       </c>
@@ -6615,6 +6900,9 @@
       <c r="D208" t="s">
         <v>465</v>
       </c>
+      <c r="G208" t="s">
+        <v>485</v>
+      </c>
       <c r="H208" t="s">
         <v>350</v>
       </c>
@@ -6635,6 +6923,9 @@
       <c r="D209" t="s">
         <v>465</v>
       </c>
+      <c r="G209" t="s">
+        <v>485</v>
+      </c>
       <c r="H209" t="s">
         <v>350</v>
       </c>
@@ -6655,6 +6946,9 @@
       <c r="D210" t="s">
         <v>465</v>
       </c>
+      <c r="G210" t="s">
+        <v>485</v>
+      </c>
       <c r="H210" t="s">
         <v>350</v>
       </c>
@@ -6675,6 +6969,9 @@
       <c r="D211" t="s">
         <v>465</v>
       </c>
+      <c r="G211" t="s">
+        <v>485</v>
+      </c>
       <c r="H211" t="s">
         <v>350</v>
       </c>
@@ -6695,6 +6992,9 @@
       <c r="D212" t="s">
         <v>465</v>
       </c>
+      <c r="G212" t="s">
+        <v>485</v>
+      </c>
       <c r="H212" t="s">
         <v>350</v>
       </c>
@@ -6715,6 +7015,9 @@
       <c r="D213" t="s">
         <v>465</v>
       </c>
+      <c r="G213" t="s">
+        <v>485</v>
+      </c>
       <c r="H213" t="s">
         <v>350</v>
       </c>
@@ -6735,6 +7038,9 @@
       <c r="D214" t="s">
         <v>465</v>
       </c>
+      <c r="G214" t="s">
+        <v>485</v>
+      </c>
       <c r="H214" t="s">
         <v>350</v>
       </c>
@@ -6755,6 +7061,9 @@
       <c r="D215" t="s">
         <v>465</v>
       </c>
+      <c r="G215" t="s">
+        <v>485</v>
+      </c>
       <c r="H215" t="s">
         <v>350</v>
       </c>
@@ -6775,6 +7084,9 @@
       <c r="D216" t="s">
         <v>465</v>
       </c>
+      <c r="G216" t="s">
+        <v>485</v>
+      </c>
       <c r="H216" t="s">
         <v>350</v>
       </c>
@@ -6795,6 +7107,9 @@
       <c r="D217" t="s">
         <v>465</v>
       </c>
+      <c r="G217" t="s">
+        <v>485</v>
+      </c>
       <c r="H217" t="s">
         <v>350</v>
       </c>
@@ -6815,6 +7130,9 @@
       <c r="D218" t="s">
         <v>465</v>
       </c>
+      <c r="G218" t="s">
+        <v>485</v>
+      </c>
       <c r="H218" t="s">
         <v>350</v>
       </c>
@@ -6835,6 +7153,9 @@
       <c r="D219" t="s">
         <v>465</v>
       </c>
+      <c r="G219" t="s">
+        <v>485</v>
+      </c>
       <c r="H219" t="s">
         <v>350</v>
       </c>
@@ -6855,6 +7176,9 @@
       <c r="D220" t="s">
         <v>465</v>
       </c>
+      <c r="G220" t="s">
+        <v>485</v>
+      </c>
       <c r="H220" t="s">
         <v>350</v>
       </c>
@@ -6875,6 +7199,9 @@
       <c r="D221" t="s">
         <v>465</v>
       </c>
+      <c r="G221" t="s">
+        <v>485</v>
+      </c>
       <c r="H221" t="s">
         <v>350</v>
       </c>
@@ -6895,6 +7222,9 @@
       <c r="D222" t="s">
         <v>465</v>
       </c>
+      <c r="G222" t="s">
+        <v>485</v>
+      </c>
       <c r="H222" t="s">
         <v>350</v>
       </c>
@@ -6915,6 +7245,9 @@
       <c r="D223" t="s">
         <v>465</v>
       </c>
+      <c r="G223" t="s">
+        <v>485</v>
+      </c>
       <c r="H223" t="s">
         <v>350</v>
       </c>
@@ -6935,6 +7268,9 @@
       <c r="D224" t="s">
         <v>465</v>
       </c>
+      <c r="G224" t="s">
+        <v>485</v>
+      </c>
       <c r="H224" t="s">
         <v>350</v>
       </c>
@@ -6955,6 +7291,9 @@
       <c r="D225" t="s">
         <v>465</v>
       </c>
+      <c r="G225" t="s">
+        <v>485</v>
+      </c>
       <c r="H225" t="s">
         <v>350</v>
       </c>
@@ -6975,6 +7314,9 @@
       <c r="D226" t="s">
         <v>465</v>
       </c>
+      <c r="G226" t="s">
+        <v>485</v>
+      </c>
       <c r="H226" t="s">
         <v>350</v>
       </c>
@@ -6995,6 +7337,9 @@
       <c r="D227" t="s">
         <v>465</v>
       </c>
+      <c r="G227" t="s">
+        <v>485</v>
+      </c>
       <c r="H227" t="s">
         <v>350</v>
       </c>
@@ -7015,6 +7360,9 @@
       <c r="D228" t="s">
         <v>465</v>
       </c>
+      <c r="G228" t="s">
+        <v>485</v>
+      </c>
       <c r="H228" t="s">
         <v>350</v>
       </c>
@@ -7035,6 +7383,9 @@
       <c r="D229" t="s">
         <v>465</v>
       </c>
+      <c r="G229" t="s">
+        <v>485</v>
+      </c>
       <c r="H229" t="s">
         <v>350</v>
       </c>
@@ -7055,6 +7406,9 @@
       <c r="D230" t="s">
         <v>371</v>
       </c>
+      <c r="G230" t="s">
+        <v>486</v>
+      </c>
       <c r="H230" t="s">
         <v>350</v>
       </c>
@@ -7075,6 +7429,9 @@
       <c r="D231" t="s">
         <v>371</v>
       </c>
+      <c r="G231" t="s">
+        <v>486</v>
+      </c>
       <c r="H231" t="s">
         <v>350</v>
       </c>
@@ -7095,6 +7452,9 @@
       <c r="D232" t="s">
         <v>371</v>
       </c>
+      <c r="G232" t="s">
+        <v>486</v>
+      </c>
       <c r="H232" t="s">
         <v>350</v>
       </c>
@@ -7115,6 +7475,9 @@
       <c r="D233" t="s">
         <v>371</v>
       </c>
+      <c r="G233" t="s">
+        <v>486</v>
+      </c>
       <c r="H233" t="s">
         <v>350</v>
       </c>
@@ -7135,6 +7498,9 @@
       <c r="D234" t="s">
         <v>371</v>
       </c>
+      <c r="G234" t="s">
+        <v>486</v>
+      </c>
       <c r="H234" t="s">
         <v>350</v>
       </c>
@@ -7155,6 +7521,9 @@
       <c r="D235" t="s">
         <v>371</v>
       </c>
+      <c r="G235" t="s">
+        <v>486</v>
+      </c>
       <c r="H235" t="s">
         <v>350</v>
       </c>
@@ -7175,6 +7544,9 @@
       <c r="D236" t="s">
         <v>371</v>
       </c>
+      <c r="G236" t="s">
+        <v>486</v>
+      </c>
       <c r="H236" t="s">
         <v>350</v>
       </c>
@@ -7195,6 +7567,9 @@
       <c r="D237" t="s">
         <v>371</v>
       </c>
+      <c r="G237" t="s">
+        <v>486</v>
+      </c>
       <c r="H237" t="s">
         <v>350</v>
       </c>
@@ -7215,6 +7590,9 @@
       <c r="D238" t="s">
         <v>371</v>
       </c>
+      <c r="G238" t="s">
+        <v>486</v>
+      </c>
       <c r="H238" t="s">
         <v>350</v>
       </c>
@@ -7235,6 +7613,9 @@
       <c r="D239" t="s">
         <v>371</v>
       </c>
+      <c r="G239" t="s">
+        <v>486</v>
+      </c>
       <c r="H239" t="s">
         <v>350</v>
       </c>
@@ -7255,6 +7636,9 @@
       <c r="D240" t="s">
         <v>371</v>
       </c>
+      <c r="G240" t="s">
+        <v>486</v>
+      </c>
       <c r="H240" t="s">
         <v>350</v>
       </c>
@@ -7275,6 +7659,9 @@
       <c r="D241" t="s">
         <v>371</v>
       </c>
+      <c r="G241" t="s">
+        <v>486</v>
+      </c>
       <c r="H241" t="s">
         <v>350</v>
       </c>
@@ -7295,6 +7682,9 @@
       <c r="D242" t="s">
         <v>371</v>
       </c>
+      <c r="G242" t="s">
+        <v>486</v>
+      </c>
       <c r="H242" t="s">
         <v>350</v>
       </c>
@@ -7315,6 +7705,9 @@
       <c r="D243" t="s">
         <v>371</v>
       </c>
+      <c r="G243" t="s">
+        <v>486</v>
+      </c>
       <c r="H243" t="s">
         <v>350</v>
       </c>
@@ -7335,6 +7728,9 @@
       <c r="D244" t="s">
         <v>371</v>
       </c>
+      <c r="G244" t="s">
+        <v>486</v>
+      </c>
       <c r="H244" t="s">
         <v>350</v>
       </c>
@@ -7355,6 +7751,9 @@
       <c r="D245" t="s">
         <v>371</v>
       </c>
+      <c r="G245" t="s">
+        <v>486</v>
+      </c>
       <c r="H245" t="s">
         <v>350</v>
       </c>
@@ -7375,6 +7774,9 @@
       <c r="D246" t="s">
         <v>371</v>
       </c>
+      <c r="G246" t="s">
+        <v>486</v>
+      </c>
       <c r="H246" t="s">
         <v>350</v>
       </c>
@@ -7395,6 +7797,9 @@
       <c r="D247" t="s">
         <v>371</v>
       </c>
+      <c r="G247" t="s">
+        <v>486</v>
+      </c>
       <c r="H247" t="s">
         <v>350</v>
       </c>
@@ -7415,6 +7820,9 @@
       <c r="D248" t="s">
         <v>371</v>
       </c>
+      <c r="G248" t="s">
+        <v>486</v>
+      </c>
       <c r="H248" t="s">
         <v>350</v>
       </c>
@@ -7435,6 +7843,9 @@
       <c r="D249" t="s">
         <v>371</v>
       </c>
+      <c r="G249" t="s">
+        <v>486</v>
+      </c>
       <c r="H249" t="s">
         <v>350</v>
       </c>
@@ -7455,6 +7866,9 @@
       <c r="D250" t="s">
         <v>371</v>
       </c>
+      <c r="G250" t="s">
+        <v>486</v>
+      </c>
       <c r="H250" t="s">
         <v>350</v>
       </c>
@@ -7475,6 +7889,9 @@
       <c r="D251" t="s">
         <v>371</v>
       </c>
+      <c r="G251" t="s">
+        <v>486</v>
+      </c>
       <c r="H251" t="s">
         <v>350</v>
       </c>
@@ -7495,6 +7912,9 @@
       <c r="D252" t="s">
         <v>371</v>
       </c>
+      <c r="G252" t="s">
+        <v>486</v>
+      </c>
       <c r="H252" t="s">
         <v>350</v>
       </c>
@@ -7515,6 +7935,9 @@
       <c r="D253" t="s">
         <v>371</v>
       </c>
+      <c r="G253" t="s">
+        <v>486</v>
+      </c>
       <c r="H253" t="s">
         <v>350</v>
       </c>
@@ -7535,6 +7958,9 @@
       <c r="D254" t="s">
         <v>371</v>
       </c>
+      <c r="G254" t="s">
+        <v>486</v>
+      </c>
       <c r="H254" t="s">
         <v>350</v>
       </c>
@@ -7555,6 +7981,9 @@
       <c r="D255" t="s">
         <v>371</v>
       </c>
+      <c r="G255" t="s">
+        <v>486</v>
+      </c>
       <c r="H255" t="s">
         <v>350</v>
       </c>
@@ -7575,6 +8004,9 @@
       <c r="D256" t="s">
         <v>371</v>
       </c>
+      <c r="G256" t="s">
+        <v>486</v>
+      </c>
       <c r="H256" t="s">
         <v>350</v>
       </c>
@@ -7595,6 +8027,9 @@
       <c r="D257" t="s">
         <v>371</v>
       </c>
+      <c r="G257" t="s">
+        <v>486</v>
+      </c>
       <c r="H257" t="s">
         <v>350</v>
       </c>
@@ -7615,6 +8050,9 @@
       <c r="D258" t="s">
         <v>371</v>
       </c>
+      <c r="G258" t="s">
+        <v>486</v>
+      </c>
       <c r="H258" t="s">
         <v>350</v>
       </c>
@@ -7635,6 +8073,9 @@
       <c r="D259" t="s">
         <v>371</v>
       </c>
+      <c r="G259" t="s">
+        <v>486</v>
+      </c>
       <c r="H259" t="s">
         <v>350</v>
       </c>
@@ -7654,6 +8095,9 @@
       </c>
       <c r="D260" t="s">
         <v>371</v>
+      </c>
+      <c r="G260" t="s">
+        <v>486</v>
       </c>
       <c r="H260" t="s">
         <v>350</v>

</xml_diff>